<commit_message>
add new checks for values
</commit_message>
<xml_diff>
--- a/membersOf_v2.xlsx
+++ b/membersOf_v2.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
+    <workbookView xWindow="240" yWindow="255" windowWidth="20115" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$151</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="190">
   <si>
     <t>AltCats</t>
   </si>
@@ -529,6 +529,66 @@
   </si>
   <si>
     <t xml:space="preserve">, </t>
+  </si>
+  <si>
+    <t>functions.add(new Function(</t>
+  </si>
+  <si>
+    <t>));</t>
+  </si>
+  <si>
+    <t>CompatibleProducts</t>
+  </si>
+  <si>
+    <t>COALESCE()</t>
+  </si>
+  <si>
+    <t>You can invoke nothing on it</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>Data[\"\"]</t>
+  </si>
+  <si>
+    <t>Gtin</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>HasValue</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>ProductPackage</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>IsBiggerThan()</t>
+  </si>
+  <si>
+    <t>BulletFeatures[]</t>
+  </si>
+  <si>
+    <t>Ksp[]</t>
+  </si>
+  <si>
+    <t>\"\"</t>
   </si>
 </sst>
 </file>
@@ -544,7 +604,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -563,6 +623,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -576,13 +648,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -884,11 +959,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P135"/>
+  <dimension ref="A1:R151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I113" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P135"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -909,7 +982,7 @@
     <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>136</v>
       </c>
@@ -955,11 +1028,17 @@
       <c r="O1" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="8" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q1" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -1000,17 +1079,17 @@
         <f t="shared" si="0"/>
         <v>""</v>
       </c>
-      <c r="P2" t="str">
-        <f>SUBSTITUTE(CONCATENATE(I2,$P$1,J2,$P$1,K2,$P$1,L2,$P$1,M2,$P$1,N2,$P$1,O2),", """"","")</f>
-        <v>"Main", "AlternativeCategory", "ProductCategories"</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P2" s="7" t="str">
+        <f>SUBSTITUTE(CONCATENATE($Q$1,I2,$P$1,J2,$P$1,K2,$P$1,L2,$P$1,M2,$P$1,N2,$P$1,O2,$R$1),", """"","")</f>
+        <v>functions.add(new Function("Main", "AlternativeCategory", "ProductCategories"));</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
-        <v>156</v>
+      <c r="B3" s="4" t="s">
+        <v>128</v>
       </c>
       <c r="C3" t="s">
         <v>156</v>
@@ -1023,6 +1102,9 @@
       </c>
       <c r="F3" s="2" t="s">
         <v>127</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>165</v>
       </c>
       <c r="I3" s="5" t="str">
         <f t="shared" ref="I3:I66" si="1">CONCATENATE("""",A3,"""")</f>
@@ -1030,7 +1112,7 @@
       </c>
       <c r="J3" t="str">
         <f t="shared" ref="J3:J66" si="2">CONCATENATE("""",B3,"""")</f>
-        <v>"Boolean"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" ref="K3:K66" si="3">CONCATENATE("""",D3,"""")</f>
@@ -1046,23 +1128,23 @@
       </c>
       <c r="N3" t="str">
         <f t="shared" ref="N3:N66" si="6">CONCATENATE("""",G3,"""")</f>
-        <v>""</v>
+        <v>"String"</v>
       </c>
       <c r="O3" t="str">
         <f t="shared" ref="O3:O66" si="7">CONCATENATE("""",H3,"""")</f>
         <v>""</v>
       </c>
-      <c r="P3" t="str">
-        <f t="shared" ref="P3:P66" si="8">SUBSTITUTE(CONCATENATE(I3,$P$1,J3,$P$1,K3,$P$1,L3,$P$1,M3,$P$1,N3,$P$1,O3),", """"","")</f>
-        <v>"HasText", "Boolean", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P3" s="7" t="str">
+        <f t="shared" ref="P3:P66" si="8">SUBSTITUTE(CONCATENATE($Q$1,I3,$P$1,J3,$P$1,K3,$P$1,L3,$P$1,M3,$P$1,N3,$P$1,O3,$R$1),", """"","")</f>
+        <v>functions.add(new Function("HasText", "ExpressionResultLiteral", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "String"));</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" t="s">
-        <v>156</v>
+      <c r="B4" s="4" t="s">
+        <v>128</v>
       </c>
       <c r="C4" t="s">
         <v>156</v>
@@ -1075,6 +1157,9 @@
       </c>
       <c r="F4" s="2" t="s">
         <v>127</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>165</v>
       </c>
       <c r="I4" s="5" t="str">
         <f t="shared" si="1"/>
@@ -1082,7 +1167,7 @@
       </c>
       <c r="J4" t="str">
         <f t="shared" si="2"/>
-        <v>"Boolean"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="3"/>
@@ -1098,23 +1183,23 @@
       </c>
       <c r="N4" t="str">
         <f t="shared" si="6"/>
-        <v>""</v>
+        <v>"String"</v>
       </c>
       <c r="O4" t="str">
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P4" t="str">
+      <c r="P4" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"IsEmpty", "Boolean", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>functions.add(new Function("IsEmpty", "ExpressionResultLiteral", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "String"));</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B5" t="s">
-        <v>156</v>
+      <c r="B5" s="4" t="s">
+        <v>128</v>
       </c>
       <c r="C5" t="s">
         <v>156</v>
@@ -1128,7 +1213,7 @@
       </c>
       <c r="J5" t="str">
         <f t="shared" si="2"/>
-        <v>"Boolean"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="3"/>
@@ -1150,12 +1235,12 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P5" t="str">
+      <c r="P5" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"IsDescendantOf()", "Boolean", "AlternativeCategory"</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>functions.add(new Function("IsDescendantOf()", "ExpressionResultLiteral", "AlternativeCategory"));</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -1196,12 +1281,12 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P6" t="str">
+      <c r="P6" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"LaunchDate", "DateTime", "Sku"</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+        <v>functions.add(new Function("LaunchDate", "DateTime", "Sku"));</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>84</v>
       </c>
@@ -1242,17 +1327,17 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P7" t="str">
+      <c r="P7" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"GetDateTime()", "DateTimeOffset", "SystemObject"</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+        <v>functions.add(new Function("GetDateTime()", "DateTimeOffset", "SystemObject"));</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
-        <v>159</v>
+      <c r="B8" s="4" t="s">
+        <v>162</v>
       </c>
       <c r="C8" t="s">
         <v>159</v>
@@ -1275,7 +1360,7 @@
       </c>
       <c r="J8" t="str">
         <f t="shared" si="2"/>
-        <v>"Decimal"</v>
+        <v>"Int32"</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="3"/>
@@ -1297,17 +1382,17 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P8" t="str">
+      <c r="P8" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Count", "Decimal", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "PdmMultivalueAttribute"</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+        <v>functions.add(new Function("Count", "Int32", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "PdmMultivalueAttribute"));</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B9" t="s">
-        <v>159</v>
+      <c r="B9" s="4" t="s">
+        <v>162</v>
       </c>
       <c r="C9" t="s">
         <v>159</v>
@@ -1324,7 +1409,7 @@
       </c>
       <c r="J9" t="str">
         <f t="shared" si="2"/>
-        <v>"Decimal"</v>
+        <v>"Int32"</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="3"/>
@@ -1346,12 +1431,12 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P9" t="str">
+      <c r="P9" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Total", "Decimal", "PdmMultivalueAttribute", "PdmRepeatingAttribute"</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+        <v>functions.add(new Function("Total", "Int32", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -1392,12 +1477,12 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P10" t="str">
+      <c r="P10" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"BestImage", "DigitalContentItem", "DigitalContent"</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+        <v>functions.add(new Function("BestImage", "DigitalContentItem", "DigitalContent"));</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -1438,12 +1523,12 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P11" t="str">
+      <c r="P11" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"BoxContents", "DigitalContentItem", "DigitalContent"</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+        <v>functions.add(new Function("BoxContents", "DigitalContentItem", "DigitalContent"));</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
@@ -1484,12 +1569,12 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P12" t="str">
+      <c r="P12" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"KeySellingPoints", "DigitalContentItem", "DigitalContent"</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+        <v>functions.add(new Function("KeySellingPoints", "DigitalContentItem", "DigitalContent"));</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>30</v>
       </c>
@@ -1530,12 +1615,12 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P13" t="str">
+      <c r="P13" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Ksp", "DigitalContentItem", "DigitalContent"</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <v>functions.add(new Function("Ksp", "DigitalContentItem", "DigitalContent"));</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
@@ -1576,12 +1661,12 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P14" t="str">
+      <c r="P14" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"MarketingText", "DigitalContentItem", "DigitalContent"</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+        <v>functions.add(new Function("MarketingText", "DigitalContentItem", "DigitalContent"));</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -1622,12 +1707,12 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P15" t="str">
+      <c r="P15" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Msds", "DigitalContentItem", "DigitalContent"</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+        <v>functions.add(new Function("Msds", "DigitalContentItem", "DigitalContent"));</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>47</v>
       </c>
@@ -1668,9 +1753,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P16" t="str">
+      <c r="P16" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"ProductFeatures", "DigitalContentItem", "DigitalContent"</v>
+        <v>functions.add(new Function("ProductFeatures", "DigitalContentItem", "DigitalContent"));</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -1714,9 +1799,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P17" t="str">
+      <c r="P17" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"ProductSheet", "DigitalContentItem", "DigitalContent"</v>
+        <v>functions.add(new Function("ProductSheet", "DigitalContentItem", "DigitalContent"));</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -1760,9 +1845,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P18" t="str">
+      <c r="P18" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"QuickStartGuide", "DigitalContentItem", "DigitalContent"</v>
+        <v>functions.add(new Function("QuickStartGuide", "DigitalContentItem", "DigitalContent"));</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -1806,9 +1891,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P19" t="str">
+      <c r="P19" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Thumbnail", "DigitalContentItem", "DigitalContent"</v>
+        <v>functions.add(new Function("Thumbnail", "DigitalContentItem", "DigitalContent"));</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -1852,9 +1937,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P20" t="str">
+      <c r="P20" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"UserManual", "DigitalContentItem", "DigitalContent"</v>
+        <v>functions.add(new Function("UserManual", "DigitalContentItem", "DigitalContent"));</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -1898,17 +1983,17 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P21" t="str">
+      <c r="P21" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Distinct", "ExpressionResult", "ExpressionResultList"</v>
+        <v>functions.add(new Function("Distinct", "ExpressionResult", "ExpressionResultList"));</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B22" t="s">
-        <v>160</v>
+      <c r="B22" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C22" t="s">
         <v>160</v>
@@ -1922,7 +2007,7 @@
       </c>
       <c r="J22" t="str">
         <f t="shared" si="2"/>
-        <v>"ExpressionResult"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K22" t="str">
         <f t="shared" si="3"/>
@@ -1944,9 +2029,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P22" t="str">
+      <c r="P22" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Min()", "ExpressionResult", "ExpressionResultList"</v>
+        <v>functions.add(new Function("Min()", "ExpressionResultLiteral", "ExpressionResultList"));</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -1990,17 +2075,17 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P23" t="str">
+      <c r="P23" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"MinMax()", "ExpressionResult", "ExpressionResultList"</v>
+        <v>functions.add(new Function("MinMax()", "ExpressionResult", "ExpressionResultList"));</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B24" t="s">
-        <v>160</v>
+      <c r="B24" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C24" t="s">
         <v>160</v>
@@ -2014,7 +2099,7 @@
       </c>
       <c r="J24" t="str">
         <f t="shared" si="2"/>
-        <v>"ExpressionResult"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K24" t="str">
         <f t="shared" si="3"/>
@@ -2036,17 +2121,17 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P24" t="str">
+      <c r="P24" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Max()", "ExpressionResult", "ExpressionResultList"</v>
+        <v>functions.add(new Function("Max()", "ExpressionResultLiteral", "ExpressionResultList"));</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B25" t="s">
-        <v>160</v>
+      <c r="B25" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C25" t="s">
         <v>160</v>
@@ -2060,7 +2145,7 @@
       </c>
       <c r="J25" t="str">
         <f t="shared" si="2"/>
-        <v>"ExpressionResult"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K25" t="str">
         <f t="shared" si="3"/>
@@ -2082,17 +2167,17 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P25" t="str">
+      <c r="P25" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Last()", "ExpressionResult", "ExpressionResultList"</v>
+        <v>functions.add(new Function("Last()", "ExpressionResultLiteral", "ExpressionResultList"));</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B26" t="s">
-        <v>160</v>
+      <c r="B26" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C26" t="s">
         <v>160</v>
@@ -2106,7 +2191,7 @@
       </c>
       <c r="J26" t="str">
         <f t="shared" si="2"/>
-        <v>"ExpressionResult"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K26" t="str">
         <f t="shared" si="3"/>
@@ -2128,9 +2213,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P26" t="str">
+      <c r="P26" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"FlattenWithAnd()", "ExpressionResult", "ExpressionResultList"</v>
+        <v>functions.add(new Function("FlattenWithAnd()", "ExpressionResultLiteral", "ExpressionResultList"));</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -2180,17 +2265,17 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P27" t="str">
+      <c r="P27" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"HtmlEncode()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("HtmlEncode()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B28" t="s">
-        <v>160</v>
+      <c r="B28" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C28" t="s">
         <v>160</v>
@@ -2204,7 +2289,7 @@
       </c>
       <c r="J28" t="str">
         <f t="shared" si="2"/>
-        <v>"ExpressionResult"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K28" t="str">
         <f t="shared" si="3"/>
@@ -2226,9 +2311,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P28" t="str">
+      <c r="P28" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"First()", "ExpressionResult", "ExpressionResultList"</v>
+        <v>functions.add(new Function("First()", "ExpressionResultLiteral", "ExpressionResultList"));</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -2272,9 +2357,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P29" t="str">
+      <c r="P29" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"DiscardNulls()", "ExpressionResult", "ExpressionResultList"</v>
+        <v>functions.add(new Function("DiscardNulls()", "ExpressionResult", "ExpressionResultList"));</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -2324,9 +2409,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P30" t="str">
+      <c r="P30" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"ExtractDecimals()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("ExtractDecimals()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -2376,9 +2461,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P31" t="str">
+      <c r="P31" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"ToLower()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("ToLower()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -2428,9 +2513,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P32" t="str">
+      <c r="P32" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"ToLowerFirstChar()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("ToLowerFirstChar()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -2480,9 +2565,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P33" t="str">
+      <c r="P33" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"ToTitleCase()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("ToTitleCase()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -2532,9 +2617,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P34" t="str">
+      <c r="P34" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"ToUpper()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("ToUpper()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -2584,9 +2669,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P35" t="str">
+      <c r="P35" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"ToUpperFirstChar()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("ToUpperFirstChar()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -2636,9 +2721,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P36" t="str">
+      <c r="P36" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Erase()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("Erase()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -2688,17 +2773,17 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P37" t="str">
+      <c r="P37" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"EraseTextSurroundedBy()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("EraseTextSurroundedBy()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B38" t="s">
-        <v>160</v>
+      <c r="B38" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C38" t="s">
         <v>160</v>
@@ -2712,7 +2797,7 @@
       </c>
       <c r="J38" t="str">
         <f t="shared" si="2"/>
-        <v>"ExpressionResult"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K38" t="str">
         <f t="shared" si="3"/>
@@ -2734,17 +2819,17 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P38" t="str">
+      <c r="P38" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"GetLine()", "ExpressionResult", "Specs"</v>
+        <v>functions.add(new Function("GetLine()", "ExpressionResultLiteral", "Specs"));</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B39" t="s">
-        <v>160</v>
+      <c r="B39" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C39" t="s">
         <v>160</v>
@@ -2758,7 +2843,7 @@
       </c>
       <c r="J39" t="str">
         <f t="shared" si="2"/>
-        <v>"ExpressionResult"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K39" t="str">
         <f t="shared" si="3"/>
@@ -2780,17 +2865,17 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P39" t="str">
+      <c r="P39" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"GetLineBody()", "ExpressionResult", "Specs"</v>
+        <v>functions.add(new Function("GetLineBody()", "ExpressionResultLiteral", "Specs"));</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B40" t="s">
-        <v>160</v>
+      <c r="B40" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C40" t="s">
         <v>160</v>
@@ -2804,7 +2889,7 @@
       </c>
       <c r="J40" t="str">
         <f t="shared" si="2"/>
-        <v>"ExpressionResult"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K40" t="str">
         <f t="shared" si="3"/>
@@ -2826,9 +2911,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P40" t="str">
+      <c r="P40" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Flatten()", "ExpressionResult", "ExpressionResultList"</v>
+        <v>functions.add(new Function("Flatten()", "ExpressionResultLiteral", "ExpressionResultList"));</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -2878,9 +2963,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P41" t="str">
+      <c r="P41" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"IfLike()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("IfLike()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -2930,9 +3015,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P42" t="str">
+      <c r="P42" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"IfLongerThan()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("IfLongerThan()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -2954,6 +3039,9 @@
       <c r="F43" s="2" t="s">
         <v>127</v>
       </c>
+      <c r="G43" s="6" t="s">
+        <v>162</v>
+      </c>
       <c r="I43" s="5" t="str">
         <f t="shared" si="1"/>
         <v>"Pluralize()"</v>
@@ -2976,15 +3064,15 @@
       </c>
       <c r="N43" t="str">
         <f t="shared" si="6"/>
-        <v>""</v>
+        <v>"Int32"</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P43" t="str">
+      <c r="P43" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Pluralize()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("Pluralize()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "Int32"));</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -3006,6 +3094,9 @@
       <c r="F44" s="2" t="s">
         <v>127</v>
       </c>
+      <c r="G44" s="6" t="s">
+        <v>165</v>
+      </c>
       <c r="I44" s="5" t="str">
         <f t="shared" si="1"/>
         <v>"Postfix()"</v>
@@ -3028,15 +3119,15 @@
       </c>
       <c r="N44" t="str">
         <f t="shared" si="6"/>
-        <v>""</v>
+        <v>"String"</v>
       </c>
       <c r="O44" t="str">
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P44" t="str">
+      <c r="P44" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Postfix()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("Postfix()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "String"));</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -3058,6 +3149,9 @@
       <c r="F45" s="2" t="s">
         <v>127</v>
       </c>
+      <c r="G45" s="6" t="s">
+        <v>165</v>
+      </c>
       <c r="I45" s="5" t="str">
         <f t="shared" si="1"/>
         <v>"Prefix()"</v>
@@ -3080,15 +3174,15 @@
       </c>
       <c r="N45" t="str">
         <f t="shared" si="6"/>
-        <v>""</v>
+        <v>"String"</v>
       </c>
       <c r="O45" t="str">
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P45" t="str">
+      <c r="P45" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Prefix()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("Prefix()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "String"));</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -3138,9 +3232,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P46" t="str">
+      <c r="P46" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"RegexReplace()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("RegexReplace()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -3190,9 +3284,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P47" t="str">
+      <c r="P47" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Replace()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("Replace()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -3214,6 +3308,9 @@
       <c r="F48" s="2" t="s">
         <v>127</v>
       </c>
+      <c r="G48" s="6" t="s">
+        <v>165</v>
+      </c>
       <c r="I48" s="5" t="str">
         <f t="shared" si="1"/>
         <v>"Shorten()"</v>
@@ -3236,23 +3333,23 @@
       </c>
       <c r="N48" t="str">
         <f t="shared" si="6"/>
-        <v>""</v>
+        <v>"String"</v>
       </c>
       <c r="O48" t="str">
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P48" t="str">
+      <c r="P48" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Shorten()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("Shorten()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "String"));</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B49" t="s">
-        <v>160</v>
+      <c r="B49" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="C49" t="s">
         <v>160</v>
@@ -3272,7 +3369,7 @@
       </c>
       <c r="J49" t="str">
         <f t="shared" si="2"/>
-        <v>"ExpressionResult"</v>
+        <v>"ExpressionResultList"</v>
       </c>
       <c r="K49" t="str">
         <f t="shared" si="3"/>
@@ -3294,9 +3391,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P49" t="str">
+      <c r="P49" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Split()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("Split()", "ExpressionResultList", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
@@ -3340,9 +3437,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P50" t="str">
+      <c r="P50" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"UseSeparators()", "ExpressionResult", "ExpressionResultList"</v>
+        <v>functions.add(new Function("UseSeparators()", "ExpressionResult", "ExpressionResultList"));</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
@@ -3392,9 +3489,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P51" t="str">
+      <c r="P51" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"InvariantValues", "ExpressionResultList", "PdmAttributeSet", "PdmMultivalueAttribute", "PdmRepeatingAttribute"</v>
+        <v>functions.add(new Function("InvariantValues", "ExpressionResultList", "PdmAttributeSet", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
@@ -3444,9 +3541,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P52" t="str">
+      <c r="P52" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Values", "ExpressionResultList", "PdmAttributeSet", "PdmMultivalueAttribute", "PdmRepeatingAttribute"</v>
+        <v>functions.add(new Function("Values", "ExpressionResultList", "PdmAttributeSet", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
@@ -3493,9 +3590,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P53" t="str">
+      <c r="P53" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"ValuesAndUnits", "ExpressionResultList", "PdmMultivalueAttribute", "PdmRepeatingAttribute"</v>
+        <v>functions.add(new Function("ValuesAndUnits", "ExpressionResultList", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
@@ -3542,9 +3639,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P54" t="str">
+      <c r="P54" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"ValuesAndUnitsUSM", "ExpressionResultList", "PdmMultivalueAttribute", "PdmRepeatingAttribute"</v>
+        <v>functions.add(new Function("ValuesAndUnitsUSM", "ExpressionResultList", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
@@ -3594,9 +3691,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P55" t="str">
+      <c r="P55" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"ValuesUSM", "ExpressionResultList", "PdmAttributeSet", "PdmMultivalueAttribute", "PdmRepeatingAttribute"</v>
+        <v>functions.add(new Function("ValuesUSM", "ExpressionResultList", "PdmAttributeSet", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
@@ -3640,9 +3737,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P56" t="str">
+      <c r="P56" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Format()", "ExpressionResultList", "ExpressionResultList"</v>
+        <v>functions.add(new Function("Format()", "ExpressionResultList", "ExpressionResultList"));</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
@@ -3686,9 +3783,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P57" t="str">
+      <c r="P57" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Skip()", "ExpressionResultList", "ExpressionResultList"</v>
+        <v>functions.add(new Function("Skip()", "ExpressionResultList", "ExpressionResultList"));</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
@@ -3732,9 +3829,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P58" t="str">
+      <c r="P58" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Take()", "ExpressionResultList", "ExpressionResultList"</v>
+        <v>functions.add(new Function("Take()", "ExpressionResultList", "ExpressionResultList"));</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
@@ -3784,9 +3881,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P59" t="str">
+      <c r="P59" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Where()", "ExpressionResultList", "ExpressionResultList", "PdmMultivalueAttribute", "PdmRepeatingAttribute"</v>
+        <v>functions.add(new Function("Where()", "ExpressionResultList", "ExpressionResultList", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
@@ -3836,17 +3933,17 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P60" t="str">
+      <c r="P60" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"WhereNot()", "ExpressionResultList", "ExpressionResultList", "PdmMultivalueAttribute", "PdmRepeatingAttribute"</v>
+        <v>functions.add(new Function("WhereNot()", "ExpressionResultList", "ExpressionResultList", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B61" t="s">
-        <v>161</v>
+      <c r="B61" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="C61" t="s">
         <v>161</v>
@@ -3860,7 +3957,7 @@
       </c>
       <c r="J61" t="str">
         <f t="shared" si="2"/>
-        <v>"IEnumerable`1"</v>
+        <v>"ExpressionResultList"</v>
       </c>
       <c r="K61" t="str">
         <f t="shared" si="3"/>
@@ -3882,9 +3979,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P61" t="str">
+      <c r="P61" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"BulletFeatures", "IEnumerable`1", "TemplexGenerator"</v>
+        <v>functions.add(new Function("BulletFeatures", "ExpressionResultList", "TemplexGenerator"));</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
@@ -3928,9 +4025,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P62" t="str">
+      <c r="P62" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"CategoryCodes", "IEnumerable`1", "RelatedProductList"</v>
+        <v>functions.add(new Function("CategoryCodes", "IEnumerable`1", "RelatedProductList"));</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
@@ -3974,17 +4071,17 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P63" t="str">
+      <c r="P63" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"CategoryKeys", "IEnumerable`1", "RelatedProductList"</v>
+        <v>functions.add(new Function("CategoryKeys", "IEnumerable`1", "RelatedProductList"));</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B64" t="s">
-        <v>161</v>
+      <c r="B64" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="C64" t="s">
         <v>161</v>
@@ -3998,7 +4095,7 @@
       </c>
       <c r="J64" t="str">
         <f t="shared" si="2"/>
-        <v>"IEnumerable`1"</v>
+        <v>"ExpressionResultList"</v>
       </c>
       <c r="K64" t="str">
         <f t="shared" si="3"/>
@@ -4020,9 +4117,9 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P64" t="str">
+      <c r="P64" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"Colors", "IEnumerable`1", "Sku"</v>
+        <v>functions.add(new Function("Colors", "ExpressionResultList", "Sku"));</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
@@ -4066,17 +4163,17 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P65" t="str">
+      <c r="P65" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"CustomerPns", "IEnumerable`1", "RelatedProductList"</v>
+        <v>functions.add(new Function("CustomerPns", "IEnumerable`1", "RelatedProductList"));</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B66" t="s">
-        <v>161</v>
+      <c r="B66" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="C66" t="s">
         <v>161</v>
@@ -4090,7 +4187,7 @@
       </c>
       <c r="J66" t="str">
         <f t="shared" si="2"/>
-        <v>"IEnumerable`1"</v>
+        <v>"ExpressionResultList"</v>
       </c>
       <c r="K66" t="str">
         <f t="shared" si="3"/>
@@ -4112,17 +4209,17 @@
         <f t="shared" si="7"/>
         <v>""</v>
       </c>
-      <c r="P66" t="str">
+      <c r="P66" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>"FancyColors", "IEnumerable`1", "Sku"</v>
+        <v>functions.add(new Function("FancyColors", "ExpressionResultList", "Sku"));</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B67" t="s">
-        <v>161</v>
+      <c r="B67" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="C67" t="s">
         <v>161</v>
@@ -4131,44 +4228,44 @@
         <v>130</v>
       </c>
       <c r="I67" s="5" t="str">
-        <f t="shared" ref="I67:I130" si="9">CONCATENATE("""",A67,"""")</f>
+        <f t="shared" ref="I67:I131" si="9">CONCATENATE("""",A67,"""")</f>
         <v>"InvariantColors"</v>
       </c>
       <c r="J67" t="str">
-        <f t="shared" ref="J67:J130" si="10">CONCATENATE("""",B67,"""")</f>
-        <v>"IEnumerable`1"</v>
+        <f t="shared" ref="J67:J131" si="10">CONCATENATE("""",B67,"""")</f>
+        <v>"ExpressionResultList"</v>
       </c>
       <c r="K67" t="str">
-        <f t="shared" ref="K67:K130" si="11">CONCATENATE("""",D67,"""")</f>
+        <f t="shared" ref="K67:K131" si="11">CONCATENATE("""",D67,"""")</f>
         <v>"Sku"</v>
       </c>
       <c r="L67" t="str">
-        <f t="shared" ref="L67:L130" si="12">CONCATENATE("""",E67,"""")</f>
+        <f t="shared" ref="L67:L131" si="12">CONCATENATE("""",E67,"""")</f>
         <v>""</v>
       </c>
       <c r="M67" t="str">
-        <f t="shared" ref="M67:M130" si="13">CONCATENATE("""",F67,"""")</f>
+        <f t="shared" ref="M67:M131" si="13">CONCATENATE("""",F67,"""")</f>
         <v>""</v>
       </c>
       <c r="N67" t="str">
-        <f t="shared" ref="N67:N130" si="14">CONCATENATE("""",G67,"""")</f>
+        <f t="shared" ref="N67:N131" si="14">CONCATENATE("""",G67,"""")</f>
         <v>""</v>
       </c>
       <c r="O67" t="str">
-        <f t="shared" ref="O67:O130" si="15">CONCATENATE("""",H67,"""")</f>
-        <v>""</v>
-      </c>
-      <c r="P67" t="str">
-        <f t="shared" ref="P67:P130" si="16">SUBSTITUTE(CONCATENATE(I67,$P$1,J67,$P$1,K67,$P$1,L67,$P$1,M67,$P$1,N67,$P$1,O67),", """"","")</f>
-        <v>"InvariantColors", "IEnumerable`1", "Sku"</v>
+        <f t="shared" ref="O67:O131" si="15">CONCATENATE("""",H67,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="P67" s="7" t="str">
+        <f t="shared" ref="P67:P131" si="16">SUBSTITUTE(CONCATENATE($Q$1,I67,$P$1,J67,$P$1,K67,$P$1,L67,$P$1,M67,$P$1,N67,$P$1,O67,$R$1),", """"","")</f>
+        <v>functions.add(new Function("InvariantColors", "ExpressionResultList", "Sku"));</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B68" t="s">
-        <v>161</v>
+      <c r="B68" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="C68" t="s">
         <v>161</v>
@@ -4182,7 +4279,7 @@
       </c>
       <c r="J68" t="str">
         <f t="shared" si="10"/>
-        <v>"IEnumerable`1"</v>
+        <v>"ExpressionResultList"</v>
       </c>
       <c r="K68" t="str">
         <f t="shared" si="11"/>
@@ -4204,9 +4301,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P68" t="str">
+      <c r="P68" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"Keywords", "IEnumerable`1", "Sku"</v>
+        <v>functions.add(new Function("Keywords", "ExpressionResultList", "Sku"));</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
@@ -4250,9 +4347,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P69" t="str">
+      <c r="P69" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"ManufacturerNames", "IEnumerable`1", "RelatedProductList"</v>
+        <v>functions.add(new Function("ManufacturerNames", "IEnumerable`1", "RelatedProductList"));</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
@@ -4296,9 +4393,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P70" t="str">
+      <c r="P70" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"ModelNames", "IEnumerable`1", "RelatedProductList"</v>
+        <v>functions.add(new Function("ModelNames", "IEnumerable`1", "RelatedProductList"));</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
@@ -4342,9 +4439,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P71" t="str">
+      <c r="P71" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"ProductIds", "IEnumerable`1", "RelatedProductList"</v>
+        <v>functions.add(new Function("ProductIds", "IEnumerable`1", "RelatedProductList"));</v>
       </c>
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
@@ -4388,9 +4485,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P72" t="str">
+      <c r="P72" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"ProductLineNames", "IEnumerable`1", "RelatedProductList"</v>
+        <v>functions.add(new Function("ProductLineNames", "IEnumerable`1", "RelatedProductList"));</v>
       </c>
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
@@ -4434,17 +4531,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P73" t="str">
+      <c r="P73" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"ProductNames", "IEnumerable`1", "RelatedProductList"</v>
+        <v>functions.add(new Function("ProductNames", "IEnumerable`1", "RelatedProductList"));</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B74" t="s">
-        <v>161</v>
+      <c r="B74" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="C74" t="s">
         <v>161</v>
@@ -4458,7 +4555,7 @@
       </c>
       <c r="J74" t="str">
         <f t="shared" si="10"/>
-        <v>"IEnumerable`1"</v>
+        <v>"ExpressionResultList"</v>
       </c>
       <c r="K74" t="str">
         <f t="shared" si="11"/>
@@ -4480,9 +4577,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P74" t="str">
+      <c r="P74" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"GetLines()", "IEnumerable`1", "Specs"</v>
+        <v>functions.add(new Function("GetLines()", "ExpressionResultList", "Specs"));</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
@@ -4526,9 +4623,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P75" t="str">
+      <c r="P75" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"GetAncestry()", "IEnumerable`1", "AlternativeCategory"</v>
+        <v>functions.add(new Function("GetAncestry()", "IEnumerable`1", "AlternativeCategory"));</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
@@ -4572,9 +4669,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P76" t="str">
+      <c r="P76" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"GetDescendants()", "IEnumerable`1", "AlternativeCategory"</v>
+        <v>functions.add(new Function("GetDescendants()", "IEnumerable`1", "AlternativeCategory"));</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
@@ -4618,9 +4715,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P77" t="str">
+      <c r="P77" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"CategoryKey", "Int32", "RelatedProduct"</v>
+        <v>functions.add(new Function("CategoryKey", "Int32", "RelatedProduct"));</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
@@ -4642,6 +4739,9 @@
       <c r="F78" s="2" t="s">
         <v>127</v>
       </c>
+      <c r="G78" s="4" t="s">
+        <v>184</v>
+      </c>
       <c r="I78" s="5" t="str">
         <f t="shared" si="9"/>
         <v>"Length"</v>
@@ -4664,15 +4764,15 @@
       </c>
       <c r="N78" t="str">
         <f t="shared" si="14"/>
-        <v>""</v>
+        <v>"ProductPackage"</v>
       </c>
       <c r="O78" t="str">
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P78" t="str">
+      <c r="P78" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"Length", "Int32", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("Length", "Int32", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "ProductPackage"));</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
@@ -4716,9 +4816,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P79" t="str">
+      <c r="P79" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"LineCount", "Int32", "Specs"</v>
+        <v>functions.add(new Function("LineCount", "Int32", "Specs"));</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -4762,9 +4862,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P80" t="str">
+      <c r="P80" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"NonOemAccessories", "Int32", "Sku"</v>
+        <v>functions.add(new Function("NonOemAccessories", "Int32", "Sku"));</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
@@ -4808,9 +4908,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P81" t="str">
+      <c r="P81" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"Order", "Int32", "SpecLine"</v>
+        <v>functions.add(new Function("Order", "Int32", "SpecLine"));</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
@@ -4857,9 +4957,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P82" t="str">
+      <c r="P82" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"PackQuantity", "Int32", "Sku", "RelatedProduct"</v>
+        <v>functions.add(new Function("PackQuantity", "Int32", "Sku", "RelatedProduct"));</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
@@ -4906,9 +5006,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P83" t="str">
+      <c r="P83" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"ProductId", "Int32", "Sku", "RelatedProduct"</v>
+        <v>functions.add(new Function("ProductId", "Int32", "Sku", "RelatedProduct"));</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
@@ -4952,9 +5052,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P84" t="str">
+      <c r="P84" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"AltCats", "List`1", "ProductCategories"</v>
+        <v>functions.add(new Function("AltCats", "List`1", "ProductCategories"));</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
@@ -4998,17 +5098,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P85" t="str">
+      <c r="P85" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"BestImages", "List`1", "DigitalContent"</v>
+        <v>functions.add(new Function("BestImages", "List`1", "DigitalContent"));</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B86" t="s">
-        <v>164</v>
+      <c r="B86" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="C86" t="s">
         <v>164</v>
@@ -5022,7 +5122,7 @@
       </c>
       <c r="J86" t="str">
         <f t="shared" si="10"/>
-        <v>"Nullable`1"</v>
+        <v>"ExpressionResultNumeric"</v>
       </c>
       <c r="K86" t="str">
         <f t="shared" si="11"/>
@@ -5044,17 +5144,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P86" t="str">
+      <c r="P86" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"Round()", "Nullable`1", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("Round()", "ExpressionResultNumeric", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B87" t="s">
-        <v>164</v>
+      <c r="B87" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="C87" t="s">
         <v>164</v>
@@ -5068,7 +5168,7 @@
       </c>
       <c r="J87" t="str">
         <f t="shared" si="10"/>
-        <v>"Nullable`1"</v>
+        <v>"ExpressionResultNumeric"</v>
       </c>
       <c r="K87" t="str">
         <f t="shared" si="11"/>
@@ -5090,17 +5190,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P87" t="str">
+      <c r="P87" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"AtLeast()", "Nullable`1", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("AtLeast()", "ExpressionResultNumeric", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B88" t="s">
-        <v>164</v>
+      <c r="B88" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="C88" t="s">
         <v>164</v>
@@ -5114,7 +5214,7 @@
       </c>
       <c r="J88" t="str">
         <f t="shared" si="10"/>
-        <v>"Nullable`1"</v>
+        <v>"ExpressionResultNumeric"</v>
       </c>
       <c r="K88" t="str">
         <f t="shared" si="11"/>
@@ -5136,17 +5236,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P88" t="str">
+      <c r="P88" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"AtMost()", "Nullable`1", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("AtMost()", "ExpressionResultNumeric", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B89" t="s">
-        <v>164</v>
+      <c r="B89" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="C89" t="s">
         <v>164</v>
@@ -5160,7 +5260,7 @@
       </c>
       <c r="J89" t="str">
         <f t="shared" si="10"/>
-        <v>"Nullable`1"</v>
+        <v>"ExpressionResultNumeric"</v>
       </c>
       <c r="K89" t="str">
         <f t="shared" si="11"/>
@@ -5182,9 +5282,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P89" t="str">
+      <c r="P89" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"MultiplyBy()", "Nullable`1", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("MultiplyBy()", "ExpressionResultNumeric", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
@@ -5228,9 +5328,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P90" t="str">
+      <c r="P90" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"Match()", "PdmAttributeSet", "PdmRepeatingAttribute"</v>
+        <v>functions.add(new Function("Match()", "PdmAttributeSet", "PdmRepeatingAttribute"));</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
@@ -5274,9 +5374,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P91" t="str">
+      <c r="P91" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"WhereUnit()", "PdmMultivalueAttribute", "PdmRepeatingAttribute"</v>
+        <v>functions.add(new Function("WhereUnit()", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
@@ -5320,9 +5420,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P92" t="str">
+      <c r="P92" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"WhereUnitOrValue()", "PdmMultivalueAttribute", "PdmRepeatingAttribute"</v>
+        <v>functions.add(new Function("WhereUnitOrValue()", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
       </c>
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
@@ -5366,9 +5466,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P93" t="str">
+      <c r="P93" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"WhereCategory()", "RelatedProductList", "RelatedProductList"</v>
+        <v>functions.add(new Function("WhereCategory()", "RelatedProductList", "RelatedProductList"));</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
@@ -5412,9 +5512,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P94" t="str">
+      <c r="P94" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"WhereManufacturer()", "RelatedProductList", "RelatedProductList"</v>
+        <v>functions.add(new Function("WhereManufacturer()", "RelatedProductList", "RelatedProductList"));</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
@@ -5458,9 +5558,9 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P95" t="str">
+      <c r="P95" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"WhereModelName()", "RelatedProductList", "RelatedProductList"</v>
+        <v>functions.add(new Function("WhereModelName()", "RelatedProductList", "RelatedProductList"));</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
@@ -5504,17 +5604,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P96" t="str">
+      <c r="P96" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"WhereProductLine()", "RelatedProductList", "RelatedProductList"</v>
+        <v>functions.add(new Function("WhereProductLine()", "RelatedProductList", "RelatedProductList"));</v>
       </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B97" t="s">
-        <v>165</v>
+      <c r="B97" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C97" t="s">
         <v>165</v>
@@ -5528,7 +5628,7 @@
       </c>
       <c r="J97" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K97" t="str">
         <f t="shared" si="11"/>
@@ -5550,17 +5650,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P97" t="str">
+      <c r="P97" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"Body", "String", "SpecLine"</v>
+        <v>functions.add(new Function("Body", "ExpressionResultLiteral", "SpecLine"));</v>
       </c>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B98" t="s">
-        <v>165</v>
+      <c r="B98" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C98" t="s">
         <v>165</v>
@@ -5577,7 +5677,7 @@
       </c>
       <c r="J98" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K98" t="str">
         <f t="shared" si="11"/>
@@ -5599,17 +5699,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P98" t="str">
+      <c r="P98" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"Brand", "String", "Sku", "RelatedProduct"</v>
+        <v>functions.add(new Function("Brand", "ExpressionResultLiteral", "Sku", "RelatedProduct"));</v>
       </c>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B99" t="s">
-        <v>165</v>
+      <c r="B99" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C99" t="s">
         <v>165</v>
@@ -5629,7 +5729,7 @@
       </c>
       <c r="J99" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K99" t="str">
         <f t="shared" si="11"/>
@@ -5651,17 +5751,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P99" t="str">
+      <c r="P99" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"CategoryCode", "String", "ProductCategories", "RelatedProduct", "RelatedProductList"</v>
+        <v>functions.add(new Function("CategoryCode", "ExpressionResultLiteral", "ProductCategories", "RelatedProduct", "RelatedProductList"));</v>
       </c>
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B100" t="s">
-        <v>165</v>
+      <c r="B100" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C100" t="s">
         <v>165</v>
@@ -5678,7 +5778,7 @@
       </c>
       <c r="J100" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K100" t="str">
         <f t="shared" si="11"/>
@@ -5700,17 +5800,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P100" t="str">
+      <c r="P100" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"CustomerPn", "String", "RelatedProduct", "RelatedProductList"</v>
+        <v>functions.add(new Function("CustomerPn", "ExpressionResultLiteral", "RelatedProduct", "RelatedProductList"));</v>
       </c>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B101" t="s">
-        <v>165</v>
+      <c r="B101" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C101" t="s">
         <v>165</v>
@@ -5727,7 +5827,7 @@
       </c>
       <c r="J101" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K101" t="str">
         <f t="shared" si="11"/>
@@ -5749,17 +5849,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P101" t="str">
+      <c r="P101" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"Description", "String", "Sku", "DigitalContentItem"</v>
+        <v>functions.add(new Function("Description", "ExpressionResultLiteral", "Sku", "DigitalContentItem"));</v>
       </c>
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B102" t="s">
-        <v>165</v>
+      <c r="B102" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C102" t="s">
         <v>165</v>
@@ -5779,7 +5879,7 @@
       </c>
       <c r="J102" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K102" t="str">
         <f t="shared" si="11"/>
@@ -5801,17 +5901,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P102" t="str">
+      <c r="P102" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"GroupName", "String", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute"</v>
+        <v>functions.add(new Function("GroupName", "ExpressionResultLiteral", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B103" t="s">
-        <v>165</v>
+      <c r="B103" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C103" t="s">
         <v>165</v>
@@ -5825,7 +5925,7 @@
       </c>
       <c r="J103" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K103" t="str">
         <f t="shared" si="11"/>
@@ -5847,17 +5947,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P103" t="str">
+      <c r="P103" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"Header", "String", "SpecLine"</v>
+        <v>functions.add(new Function("Header", "ExpressionResultLiteral", "SpecLine"));</v>
       </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B104" t="s">
-        <v>165</v>
+      <c r="B104" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C104" t="s">
         <v>165</v>
@@ -5877,7 +5977,7 @@
       </c>
       <c r="J104" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K104" t="str">
         <f t="shared" si="11"/>
@@ -5899,17 +5999,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P104" t="str">
+      <c r="P104" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"Invariant", "String", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute"</v>
+        <v>functions.add(new Function("Invariant", "ExpressionResultLiteral", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B105" t="s">
-        <v>165</v>
+      <c r="B105" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C105" t="s">
         <v>165</v>
@@ -5929,7 +6029,7 @@
       </c>
       <c r="J105" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K105" t="str">
         <f t="shared" si="11"/>
@@ -5951,17 +6051,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P105" t="str">
+      <c r="P105" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"InvariantUnit", "String", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute"</v>
+        <v>functions.add(new Function("InvariantUnit", "ExpressionResultLiteral", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B106" t="s">
-        <v>165</v>
+      <c r="B106" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C106" t="s">
         <v>165</v>
@@ -5975,7 +6075,7 @@
       </c>
       <c r="J106" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K106" t="str">
         <f t="shared" si="11"/>
@@ -5997,17 +6097,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P106" t="str">
+      <c r="P106" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"ItemName", "String", "Sku"</v>
+        <v>functions.add(new Function("ItemName", "ExpressionResultLiteral", "Sku"));</v>
       </c>
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B107" t="s">
-        <v>165</v>
+      <c r="B107" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C107" t="s">
         <v>165</v>
@@ -6021,7 +6121,7 @@
       </c>
       <c r="J107" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K107" t="str">
         <f t="shared" si="11"/>
@@ -6043,17 +6143,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P107" t="str">
+      <c r="P107" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"Key", "String", "AlternativeCategory"</v>
+        <v>functions.add(new Function("Key", "ExpressionResultLiteral", "AlternativeCategory"));</v>
       </c>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B108" t="s">
-        <v>165</v>
+      <c r="B108" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C108" t="s">
         <v>165</v>
@@ -6070,7 +6170,7 @@
       </c>
       <c r="J108" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K108" t="str">
         <f t="shared" si="11"/>
@@ -6092,17 +6192,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P108" t="str">
+      <c r="P108" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"Manufacturer", "String", "Sku", "RelatedProduct"</v>
+        <v>functions.add(new Function("Manufacturer", "ExpressionResultLiteral", "Sku", "RelatedProduct"));</v>
       </c>
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B109" t="s">
-        <v>165</v>
+      <c r="B109" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C109" t="s">
         <v>165</v>
@@ -6116,7 +6216,7 @@
       </c>
       <c r="J109" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K109" t="str">
         <f t="shared" si="11"/>
@@ -6138,17 +6238,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P109" t="str">
+      <c r="P109" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"MimeType", "String", "DigitalContentItem"</v>
+        <v>functions.add(new Function("MimeType", "ExpressionResultLiteral", "DigitalContentItem"));</v>
       </c>
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B110" t="s">
-        <v>165</v>
+      <c r="B110" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C110" t="s">
         <v>165</v>
@@ -6165,7 +6265,7 @@
       </c>
       <c r="J110" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K110" t="str">
         <f t="shared" si="11"/>
@@ -6187,17 +6287,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P110" t="str">
+      <c r="P110" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"ModelName", "String", "Sku", "RelatedProduct"</v>
+        <v>functions.add(new Function("ModelName", "ExpressionResultLiteral", "Sku", "RelatedProduct"));</v>
       </c>
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B111" t="s">
-        <v>165</v>
+      <c r="B111" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C111" t="s">
         <v>165</v>
@@ -6223,7 +6323,7 @@
       </c>
       <c r="J111" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K111" t="str">
         <f t="shared" si="11"/>
@@ -6245,17 +6345,17 @@
         <f t="shared" si="15"/>
         <v>"SpecSection"</v>
       </c>
-      <c r="P111" t="str">
+      <c r="P111" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"Name", "String", "Sku", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute", "SpecSection"</v>
+        <v>functions.add(new Function("Name", "ExpressionResultLiteral", "Sku", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute", "SpecSection"));</v>
       </c>
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B112" t="s">
-        <v>165</v>
+      <c r="B112" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C112" t="s">
         <v>165</v>
@@ -6272,7 +6372,7 @@
       </c>
       <c r="J112" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K112" t="str">
         <f t="shared" si="11"/>
@@ -6294,17 +6394,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P112" t="str">
+      <c r="P112" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"PartNumber", "String", "Sku", "RelatedProduct"</v>
+        <v>functions.add(new Function("PartNumber", "ExpressionResultLiteral", "Sku", "RelatedProduct"));</v>
       </c>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B113" t="s">
-        <v>165</v>
+      <c r="B113" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C113" t="s">
         <v>165</v>
@@ -6321,7 +6421,7 @@
       </c>
       <c r="J113" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K113" t="str">
         <f t="shared" si="11"/>
@@ -6343,17 +6443,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P113" t="str">
+      <c r="P113" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"ProductLine", "String", "Sku", "RelatedProduct"</v>
+        <v>functions.add(new Function("ProductLine", "ExpressionResultLiteral", "Sku", "RelatedProduct"));</v>
       </c>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B114" t="s">
-        <v>165</v>
+      <c r="B114" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C114" t="s">
         <v>165</v>
@@ -6367,7 +6467,7 @@
       </c>
       <c r="J114" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K114" t="str">
         <f t="shared" si="11"/>
@@ -6389,17 +6489,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P114" t="str">
+      <c r="P114" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"ProductType", "String", "Sku"</v>
+        <v>functions.add(new Function("ProductType", "ExpressionResultLiteral", "Sku"));</v>
       </c>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B115" t="s">
-        <v>165</v>
+      <c r="B115" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C115" t="s">
         <v>165</v>
@@ -6419,7 +6519,7 @@
       </c>
       <c r="J115" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K115" t="str">
         <f t="shared" si="11"/>
@@ -6441,17 +6541,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P115" t="str">
+      <c r="P115" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"Unit", "String", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute"</v>
+        <v>functions.add(new Function("Unit", "ExpressionResultLiteral", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
       </c>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B116" t="s">
-        <v>165</v>
+      <c r="B116" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C116" t="s">
         <v>165</v>
@@ -6471,7 +6571,7 @@
       </c>
       <c r="J116" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K116" t="str">
         <f t="shared" si="11"/>
@@ -6493,17 +6593,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P116" t="str">
+      <c r="P116" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"UnitUSM", "String", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute"</v>
+        <v>functions.add(new Function("UnitUSM", "ExpressionResultLiteral", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B117" t="s">
-        <v>165</v>
+      <c r="B117" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C117" t="s">
         <v>165</v>
@@ -6516,6 +6616,9 @@
       </c>
       <c r="F117" t="s">
         <v>133</v>
+      </c>
+      <c r="G117" s="4" t="s">
+        <v>178</v>
       </c>
       <c r="I117" s="5" t="str">
         <f t="shared" si="9"/>
@@ -6523,7 +6626,7 @@
       </c>
       <c r="J117" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K117" t="str">
         <f t="shared" si="11"/>
@@ -6539,23 +6642,23 @@
       </c>
       <c r="N117" t="str">
         <f t="shared" si="14"/>
-        <v>""</v>
+        <v>"Gtin"</v>
       </c>
       <c r="O117" t="str">
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P117" t="str">
+      <c r="P117" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"Value", "String", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute"</v>
+        <v>functions.add(new Function("Value", "ExpressionResultLiteral", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute", "Gtin"));</v>
       </c>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B118" t="s">
-        <v>165</v>
+      <c r="B118" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C118" t="s">
         <v>165</v>
@@ -6575,7 +6678,7 @@
       </c>
       <c r="J118" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K118" t="str">
         <f t="shared" si="11"/>
@@ -6597,17 +6700,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P118" t="str">
+      <c r="P118" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"ValueUSM", "String", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute"</v>
+        <v>functions.add(new Function("ValueUSM", "ExpressionResultLiteral", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
       </c>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B119" t="s">
-        <v>165</v>
+      <c r="B119" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C119" t="s">
         <v>165</v>
@@ -6621,7 +6724,7 @@
       </c>
       <c r="J119" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K119" t="str">
         <f t="shared" si="11"/>
@@ -6643,17 +6746,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P119" t="str">
+      <c r="P119" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"XmlContent", "String", "DigitalContentItem"</v>
+        <v>functions.add(new Function("XmlContent", "ExpressionResultLiteral", "DigitalContentItem"));</v>
       </c>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B120" t="s">
-        <v>165</v>
+      <c r="B120" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C120" t="s">
         <v>165</v>
@@ -6667,7 +6770,7 @@
       </c>
       <c r="J120" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K120" t="str">
         <f t="shared" si="11"/>
@@ -6689,17 +6792,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P120" t="str">
+      <c r="P120" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"ListPaths()", "String", "ProductCategories"</v>
+        <v>functions.add(new Function("ListPaths()", "ExpressionResultLiteral", "ProductCategories"));</v>
       </c>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B121" t="s">
-        <v>165</v>
+      <c r="B121" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C121" t="s">
         <v>165</v>
@@ -6713,7 +6816,7 @@
       </c>
       <c r="J121" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K121" t="str">
         <f t="shared" si="11"/>
@@ -6735,17 +6838,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P121" t="str">
+      <c r="P121" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"ListUSM()", "String", "PdmAttributeSet"</v>
+        <v>functions.add(new Function("ListUSM()", "ExpressionResultLiteral", "PdmAttributeSet"));</v>
       </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B122" t="s">
-        <v>165</v>
+      <c r="B122" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C122" t="s">
         <v>165</v>
@@ -6759,7 +6862,7 @@
       </c>
       <c r="J122" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K122" t="str">
         <f t="shared" si="11"/>
@@ -6781,17 +6884,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P122" t="str">
+      <c r="P122" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"GetFullColorDescription()", "String", "TemplexGenerator"</v>
+        <v>functions.add(new Function("GetFullColorDescription()", "ExpressionResultLiteral", "TemplexGenerator"));</v>
       </c>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B123" t="s">
-        <v>165</v>
+      <c r="B123" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C123" t="s">
         <v>165</v>
@@ -6805,7 +6908,7 @@
       </c>
       <c r="J123" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K123" t="str">
         <f t="shared" si="11"/>
@@ -6827,17 +6930,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P123" t="str">
+      <c r="P123" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"ToHtml()", "String", "DigitalContentItem"</v>
+        <v>functions.add(new Function("ToHtml()", "ExpressionResultLiteral", "DigitalContentItem"));</v>
       </c>
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B124" t="s">
-        <v>165</v>
+      <c r="B124" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C124" t="s">
         <v>165</v>
@@ -6851,7 +6954,7 @@
       </c>
       <c r="J124" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K124" t="str">
         <f t="shared" si="11"/>
@@ -6873,17 +6976,17 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P124" t="str">
+      <c r="P124" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"ToPlainText()", "String", "DigitalContentItem"</v>
+        <v>functions.add(new Function("ToPlainText()", "ExpressionResultLiteral", "DigitalContentItem"));</v>
       </c>
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B125" t="s">
-        <v>165</v>
+      <c r="B125" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="C125" t="s">
         <v>165</v>
@@ -6897,13 +7000,17 @@
       <c r="F125" s="2" t="s">
         <v>127</v>
       </c>
+      <c r="G125" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="H125" s="2"/>
       <c r="I125" s="5" t="str">
         <f t="shared" si="9"/>
         <v>"ToText()"</v>
       </c>
       <c r="J125" t="str">
         <f t="shared" si="10"/>
-        <v>"String"</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="K125" t="str">
         <f t="shared" si="11"/>
@@ -6919,15 +7026,15 @@
       </c>
       <c r="N125" t="str">
         <f t="shared" si="14"/>
-        <v>""</v>
+        <v>"DateTimeOffset"</v>
       </c>
       <c r="O125" t="str">
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P125" t="str">
+      <c r="P125" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"ToText()", "String", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"</v>
+        <v>functions.add(new Function("ToText()", "ExpressionResultLiteral", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "DateTimeOffset"));</v>
       </c>
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.25">
@@ -6971,400 +7078,1076 @@
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P126" t="str">
+      <c r="P126" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"Url", "Uri", "DigitalContentItem"</v>
+        <v>functions.add(new Function("Url", "Uri", "DigitalContentItem"));</v>
       </c>
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>147</v>
-      </c>
-      <c r="B127" t="s">
-        <v>125</v>
-      </c>
-      <c r="C127" t="s">
-        <v>125</v>
+      <c r="A127" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B127" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D127" t="s">
+        <v>138</v>
       </c>
       <c r="I127" s="5" t="str">
         <f t="shared" si="9"/>
+        <v>"CompatibleProducts"</v>
+      </c>
+      <c r="J127" t="str">
+        <f t="shared" ref="J127" si="17">CONCATENATE("""",B127,"""")</f>
+        <v>"ExpressionResultList"</v>
+      </c>
+      <c r="K127" t="str">
+        <f t="shared" ref="K127" si="18">CONCATENATE("""",D127,"""")</f>
+        <v>"Specs"</v>
+      </c>
+      <c r="L127" t="str">
+        <f t="shared" ref="L127" si="19">CONCATENATE("""",E127,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="M127" t="str">
+        <f t="shared" ref="M127" si="20">CONCATENATE("""",F127,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="N127" t="str">
+        <f t="shared" ref="N127" si="21">CONCATENATE("""",G127,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="O127" t="str">
+        <f t="shared" ref="O127" si="22">CONCATENATE("""",H127,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="P127" s="7" t="str">
+        <f t="shared" ref="P127" si="23">SUBSTITUTE(CONCATENATE($Q$1,I127,$P$1,J127,$P$1,K127,$P$1,L127,$P$1,M127,$P$1,N127,$P$1,O127,$R$1),", """"","")</f>
+        <v>functions.add(new Function("CompatibleProducts", "ExpressionResultList", "Specs"));</v>
+      </c>
+    </row>
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>147</v>
+      </c>
+      <c r="B128" t="s">
+        <v>125</v>
+      </c>
+      <c r="C128" t="s">
+        <v>125</v>
+      </c>
+      <c r="I128" s="5" t="str">
+        <f t="shared" si="9"/>
         <v>"CAT"</v>
       </c>
-      <c r="J127" t="str">
+      <c r="J128" t="str">
         <f t="shared" si="10"/>
         <v>"ProductCategories"</v>
       </c>
-      <c r="K127" t="str">
+      <c r="K128" t="str">
         <f t="shared" si="11"/>
         <v>""</v>
       </c>
-      <c r="L127" t="str">
+      <c r="L128" t="str">
         <f t="shared" si="12"/>
         <v>""</v>
       </c>
-      <c r="M127" t="str">
+      <c r="M128" t="str">
         <f t="shared" si="13"/>
         <v>""</v>
       </c>
-      <c r="N127" t="str">
+      <c r="N128" t="str">
         <f t="shared" si="14"/>
         <v>""</v>
       </c>
-      <c r="O127" t="str">
+      <c r="O128" t="str">
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P127" t="str">
+      <c r="P128" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"CAT", "ProductCategories"</v>
-      </c>
-    </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
+        <v>functions.add(new Function("CAT", "ProductCategories"));</v>
+      </c>
+    </row>
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B129" t="s">
         <v>130</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C129" t="s">
         <v>130</v>
       </c>
-      <c r="I128" s="5" t="str">
+      <c r="I129" s="5" t="str">
         <f t="shared" si="9"/>
         <v>"SKU"</v>
       </c>
-      <c r="J128" t="str">
+      <c r="J129" t="str">
         <f t="shared" si="10"/>
         <v>"Sku"</v>
       </c>
-      <c r="K128" t="str">
+      <c r="K129" t="str">
         <f t="shared" si="11"/>
         <v>""</v>
       </c>
-      <c r="L128" t="str">
+      <c r="L129" t="str">
         <f t="shared" si="12"/>
         <v>""</v>
       </c>
-      <c r="M128" t="str">
+      <c r="M129" t="str">
         <f t="shared" si="13"/>
         <v>""</v>
       </c>
-      <c r="N128" t="str">
+      <c r="N129" t="str">
         <f t="shared" si="14"/>
         <v>""</v>
       </c>
-      <c r="O128" t="str">
+      <c r="O129" t="str">
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P128" t="str">
+      <c r="P129" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"SKU", "Sku"</v>
-      </c>
-    </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
+        <v>functions.add(new Function("SKU", "Sku"));</v>
+      </c>
+    </row>
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B130" t="s">
         <v>142</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C130" t="s">
         <v>142</v>
       </c>
-      <c r="I129" s="5" t="str">
+      <c r="I130" s="5" t="str">
         <f t="shared" si="9"/>
         <v>"Request"</v>
       </c>
-      <c r="J129" t="str">
+      <c r="J130" t="str">
         <f t="shared" si="10"/>
         <v>"RelatedProduct"</v>
       </c>
-      <c r="K129" t="str">
+      <c r="K130" t="str">
         <f t="shared" si="11"/>
         <v>""</v>
       </c>
-      <c r="L129" t="str">
+      <c r="L130" t="str">
         <f t="shared" si="12"/>
         <v>""</v>
       </c>
-      <c r="M129" t="str">
+      <c r="M130" t="str">
         <f t="shared" si="13"/>
         <v>""</v>
       </c>
-      <c r="N129" t="str">
+      <c r="N130" t="str">
         <f t="shared" si="14"/>
         <v>""</v>
       </c>
-      <c r="O129" t="str">
+      <c r="O130" t="str">
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P129" t="str">
+      <c r="P130" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"Request", "RelatedProduct"</v>
-      </c>
-    </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
+        <v>functions.add(new Function("Request", "RelatedProduct"));</v>
+      </c>
+    </row>
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B131" t="s">
         <v>141</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C131" t="s">
         <v>141</v>
       </c>
-      <c r="I130" s="5" t="str">
+      <c r="I131" s="5" t="str">
         <f t="shared" si="9"/>
         <v>"ParentProducts"</v>
       </c>
-      <c r="J130" t="str">
+      <c r="J131" t="str">
         <f t="shared" si="10"/>
         <v>"RelatedProductList"</v>
       </c>
-      <c r="K130" t="str">
+      <c r="K131" t="str">
         <f t="shared" si="11"/>
         <v>""</v>
       </c>
-      <c r="L130" t="str">
+      <c r="L131" t="str">
         <f t="shared" si="12"/>
         <v>""</v>
       </c>
-      <c r="M130" t="str">
+      <c r="M131" t="str">
         <f t="shared" si="13"/>
         <v>""</v>
       </c>
-      <c r="N130" t="str">
+      <c r="N131" t="str">
         <f t="shared" si="14"/>
         <v>""</v>
       </c>
-      <c r="O130" t="str">
+      <c r="O131" t="str">
         <f t="shared" si="15"/>
         <v>""</v>
       </c>
-      <c r="P130" t="str">
+      <c r="P131" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>"ParentProducts", "RelatedProductList"</v>
-      </c>
-    </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B131" t="s">
-        <v>138</v>
-      </c>
-      <c r="C131" t="s">
-        <v>138</v>
-      </c>
-      <c r="I131" s="5" t="str">
-        <f t="shared" ref="I131:I135" si="17">CONCATENATE("""",A131,"""")</f>
-        <v>"MS"</v>
-      </c>
-      <c r="J131" t="str">
-        <f t="shared" ref="J131:J135" si="18">CONCATENATE("""",B131,"""")</f>
-        <v>"Specs"</v>
-      </c>
-      <c r="K131" t="str">
-        <f t="shared" ref="K131:K135" si="19">CONCATENATE("""",D131,"""")</f>
-        <v>""</v>
-      </c>
-      <c r="L131" t="str">
-        <f t="shared" ref="L131:L135" si="20">CONCATENATE("""",E131,"""")</f>
-        <v>""</v>
-      </c>
-      <c r="M131" t="str">
-        <f t="shared" ref="M131:M135" si="21">CONCATENATE("""",F131,"""")</f>
-        <v>""</v>
-      </c>
-      <c r="N131" t="str">
-        <f t="shared" ref="N131:N135" si="22">CONCATENATE("""",G131,"""")</f>
-        <v>""</v>
-      </c>
-      <c r="O131" t="str">
-        <f t="shared" ref="O131:O135" si="23">CONCATENATE("""",H131,"""")</f>
-        <v>""</v>
-      </c>
-      <c r="P131" t="str">
-        <f t="shared" ref="P131:P135" si="24">SUBSTITUTE(CONCATENATE(I131,$P$1,J131,$P$1,K131,$P$1,L131,$P$1,M131,$P$1,N131,$P$1,O131),", """"","")</f>
-        <v>"MS", "Specs"</v>
+        <v>functions.add(new Function("ParentProducts", "RelatedProductList"));</v>
       </c>
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B132" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C132" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="I132" s="5" t="str">
-        <f t="shared" si="17"/>
-        <v>"Sys"</v>
+        <f t="shared" ref="I132:I136" si="24">CONCATENATE("""",A132,"""")</f>
+        <v>"MS"</v>
       </c>
       <c r="J132" t="str">
-        <f t="shared" si="18"/>
-        <v>"SystemObject"</v>
+        <f t="shared" ref="J132:J137" si="25">CONCATENATE("""",B132,"""")</f>
+        <v>"Specs"</v>
       </c>
       <c r="K132" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="K132:K137" si="26">CONCATENATE("""",D132,"""")</f>
         <v>""</v>
       </c>
       <c r="L132" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="L132:L137" si="27">CONCATENATE("""",E132,"""")</f>
         <v>""</v>
       </c>
       <c r="M132" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="M132:M137" si="28">CONCATENATE("""",F132,"""")</f>
         <v>""</v>
       </c>
       <c r="N132" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="N132:N137" si="29">CONCATENATE("""",G132,"""")</f>
         <v>""</v>
       </c>
       <c r="O132" t="str">
-        <f t="shared" si="23"/>
-        <v>""</v>
-      </c>
-      <c r="P132" t="str">
-        <f t="shared" si="24"/>
-        <v>"Sys", "SystemObject"</v>
+        <f t="shared" ref="O132:O137" si="30">CONCATENATE("""",H132,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="P132" s="7" t="str">
+        <f t="shared" ref="P132:P137" si="31">SUBSTITUTE(CONCATENATE($Q$1,I132,$P$1,J132,$P$1,K132,$P$1,L132,$P$1,M132,$P$1,N132,$P$1,O132,$R$1),", """"","")</f>
+        <v>functions.add(new Function("MS", "Specs"));</v>
       </c>
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B133" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C133" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="I133" s="5" t="str">
-        <f t="shared" si="17"/>
-        <v>"DC"</v>
+        <f t="shared" si="24"/>
+        <v>"Sys"</v>
       </c>
       <c r="J133" t="str">
-        <f t="shared" si="18"/>
-        <v>"DigitalContent"</v>
+        <f t="shared" si="25"/>
+        <v>"SystemObject"</v>
       </c>
       <c r="K133" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>""</v>
       </c>
       <c r="L133" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>""</v>
       </c>
       <c r="M133" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>""</v>
       </c>
       <c r="N133" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>""</v>
       </c>
       <c r="O133" t="str">
-        <f t="shared" si="23"/>
-        <v>""</v>
-      </c>
-      <c r="P133" t="str">
-        <f t="shared" si="24"/>
-        <v>"DC", "DigitalContent"</v>
+        <f t="shared" si="30"/>
+        <v>""</v>
+      </c>
+      <c r="P133" s="7" t="str">
+        <f t="shared" si="31"/>
+        <v>functions.add(new Function("Sys", "SystemObject"));</v>
       </c>
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B134" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C134" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="I134" s="5" t="str">
-        <f t="shared" si="17"/>
-        <v>"Generator"</v>
+        <f t="shared" si="24"/>
+        <v>"DC"</v>
       </c>
       <c r="J134" t="str">
-        <f t="shared" si="18"/>
-        <v>"TemplexGenerator"</v>
+        <f t="shared" si="25"/>
+        <v>"DigitalContent"</v>
       </c>
       <c r="K134" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="26"/>
         <v>""</v>
       </c>
       <c r="L134" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="27"/>
         <v>""</v>
       </c>
       <c r="M134" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="28"/>
         <v>""</v>
       </c>
       <c r="N134" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="29"/>
         <v>""</v>
       </c>
       <c r="O134" t="str">
-        <f t="shared" si="23"/>
-        <v>""</v>
-      </c>
-      <c r="P134" t="str">
-        <f t="shared" si="24"/>
-        <v>"Generator", "TemplexGenerator"</v>
+        <f t="shared" si="30"/>
+        <v>""</v>
+      </c>
+      <c r="P134" s="7" t="str">
+        <f t="shared" si="31"/>
+        <v>functions.add(new Function("DC", "DigitalContent"));</v>
       </c>
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B135" t="s">
+        <v>140</v>
+      </c>
+      <c r="C135" t="s">
+        <v>140</v>
+      </c>
+      <c r="I135" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>"Generator"</v>
+      </c>
+      <c r="J135" t="str">
+        <f t="shared" si="25"/>
+        <v>"TemplexGenerator"</v>
+      </c>
+      <c r="K135" t="str">
+        <f t="shared" si="26"/>
+        <v>""</v>
+      </c>
+      <c r="L135" t="str">
+        <f t="shared" si="27"/>
+        <v>""</v>
+      </c>
+      <c r="M135" t="str">
+        <f t="shared" si="28"/>
+        <v>""</v>
+      </c>
+      <c r="N135" t="str">
+        <f t="shared" si="29"/>
+        <v>""</v>
+      </c>
+      <c r="O135" t="str">
+        <f t="shared" si="30"/>
+        <v>""</v>
+      </c>
+      <c r="P135" s="7" t="str">
+        <f t="shared" si="31"/>
+        <v>functions.add(new Function("Generator", "TemplexGenerator"));</v>
+      </c>
+    </row>
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B136" t="s">
         <v>138</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C136" t="s">
         <v>138</v>
       </c>
-      <c r="I135" s="5" t="str">
-        <f t="shared" si="17"/>
+      <c r="I136" s="5" t="str">
+        <f t="shared" si="24"/>
         <v>"ES"</v>
       </c>
-      <c r="J135" t="str">
-        <f t="shared" si="18"/>
+      <c r="J136" t="str">
+        <f t="shared" si="25"/>
         <v>"Specs"</v>
       </c>
-      <c r="K135" t="str">
-        <f t="shared" si="19"/>
-        <v>""</v>
-      </c>
-      <c r="L135" t="str">
-        <f t="shared" si="20"/>
-        <v>""</v>
-      </c>
-      <c r="M135" t="str">
-        <f t="shared" si="21"/>
-        <v>""</v>
-      </c>
-      <c r="N135" t="str">
-        <f t="shared" si="22"/>
-        <v>""</v>
-      </c>
-      <c r="O135" t="str">
-        <f t="shared" si="23"/>
-        <v>""</v>
-      </c>
-      <c r="P135" t="str">
-        <f t="shared" si="24"/>
-        <v>"ES", "Specs"</v>
+      <c r="K136" t="str">
+        <f t="shared" si="26"/>
+        <v>""</v>
+      </c>
+      <c r="L136" t="str">
+        <f t="shared" si="27"/>
+        <v>""</v>
+      </c>
+      <c r="M136" t="str">
+        <f t="shared" si="28"/>
+        <v>""</v>
+      </c>
+      <c r="N136" t="str">
+        <f t="shared" si="29"/>
+        <v>""</v>
+      </c>
+      <c r="O136" t="str">
+        <f t="shared" si="30"/>
+        <v>""</v>
+      </c>
+      <c r="P136" s="7" t="str">
+        <f t="shared" si="31"/>
+        <v>functions.add(new Function("ES", "Specs"));</v>
+      </c>
+    </row>
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>173</v>
+      </c>
+      <c r="B137" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="I137" s="5" t="str">
+        <f t="shared" ref="I137:I139" si="32">CONCATENATE("""",A137,"""")</f>
+        <v>"COALESCE()"</v>
+      </c>
+      <c r="J137" t="str">
+        <f t="shared" si="25"/>
+        <v>"You can invoke nothing on it"</v>
+      </c>
+      <c r="K137" t="str">
+        <f t="shared" si="26"/>
+        <v>""</v>
+      </c>
+      <c r="L137" t="str">
+        <f t="shared" si="27"/>
+        <v>""</v>
+      </c>
+      <c r="M137" t="str">
+        <f t="shared" si="28"/>
+        <v>""</v>
+      </c>
+      <c r="N137" t="str">
+        <f t="shared" si="29"/>
+        <v>""</v>
+      </c>
+      <c r="O137" t="str">
+        <f t="shared" si="30"/>
+        <v>""</v>
+      </c>
+      <c r="P137" s="7" t="str">
+        <f t="shared" si="31"/>
+        <v>functions.add(new Function("COALESCE()", "You can invoke nothing on it"));</v>
+      </c>
+    </row>
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="I138" s="5" t="str">
+        <f t="shared" ref="I138:I151" si="33">CONCATENATE("""",A138,"""")</f>
+        <v>"NOT NULL"</v>
+      </c>
+      <c r="J138" t="str">
+        <f t="shared" ref="J138:J144" si="34">CONCATENATE("""",B138,"""")</f>
+        <v>"You can invoke nothing on it"</v>
+      </c>
+      <c r="K138" t="str">
+        <f t="shared" ref="K138:K144" si="35">CONCATENATE("""",D138,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="L138" t="str">
+        <f t="shared" ref="L138:L144" si="36">CONCATENATE("""",E138,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="M138" t="str">
+        <f t="shared" ref="M138:M144" si="37">CONCATENATE("""",F138,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="N138" t="str">
+        <f t="shared" ref="N138:N144" si="38">CONCATENATE("""",G138,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="O138" t="str">
+        <f t="shared" ref="O138:O144" si="39">CONCATENATE("""",H138,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="P138" s="7" t="str">
+        <f t="shared" ref="P138:P144" si="40">SUBSTITUTE(CONCATENATE($Q$1,I138,$P$1,J138,$P$1,K138,$P$1,L138,$P$1,M138,$P$1,N138,$P$1,O138,$R$1),", """"","")</f>
+        <v>functions.add(new Function("NOT NULL", "You can invoke nothing on it"));</v>
+      </c>
+    </row>
+    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="I139" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>"NULL"</v>
+      </c>
+      <c r="J139" t="str">
+        <f t="shared" si="34"/>
+        <v>"You can invoke nothing on it"</v>
+      </c>
+      <c r="K139" t="str">
+        <f t="shared" si="35"/>
+        <v>""</v>
+      </c>
+      <c r="L139" t="str">
+        <f t="shared" si="36"/>
+        <v>""</v>
+      </c>
+      <c r="M139" t="str">
+        <f t="shared" si="37"/>
+        <v>""</v>
+      </c>
+      <c r="N139" t="str">
+        <f t="shared" si="38"/>
+        <v>""</v>
+      </c>
+      <c r="O139" t="str">
+        <f t="shared" si="39"/>
+        <v>""</v>
+      </c>
+      <c r="P139" s="7" t="str">
+        <f t="shared" si="40"/>
+        <v>functions.add(new Function("NULL", "You can invoke nothing on it"));</v>
+      </c>
+    </row>
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D140" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="I140" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>"Data[\"\"]"</v>
+      </c>
+      <c r="J140" t="str">
+        <f t="shared" si="34"/>
+        <v>"ExpressionResultLiteral"</v>
+      </c>
+      <c r="K140" t="str">
+        <f t="shared" si="35"/>
+        <v>"RelatedProduct"</v>
+      </c>
+      <c r="L140" t="str">
+        <f t="shared" si="36"/>
+        <v>""</v>
+      </c>
+      <c r="M140" t="str">
+        <f t="shared" si="37"/>
+        <v>""</v>
+      </c>
+      <c r="N140" t="str">
+        <f t="shared" si="38"/>
+        <v>""</v>
+      </c>
+      <c r="O140" t="str">
+        <f t="shared" si="39"/>
+        <v>""</v>
+      </c>
+      <c r="P140" s="7" t="str">
+        <f t="shared" si="40"/>
+        <v>functions.add(new Function("Data[\"\"]", "ExpressionResultLiteral", "RelatedProduct"));</v>
+      </c>
+    </row>
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D141" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="I141" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>"Gtin"</v>
+      </c>
+      <c r="J141" t="str">
+        <f t="shared" si="34"/>
+        <v>"Gtin"</v>
+      </c>
+      <c r="K141" t="str">
+        <f t="shared" si="35"/>
+        <v>"RelatedProduct"</v>
+      </c>
+      <c r="L141" t="str">
+        <f t="shared" si="36"/>
+        <v>""</v>
+      </c>
+      <c r="M141" t="str">
+        <f t="shared" si="37"/>
+        <v>""</v>
+      </c>
+      <c r="N141" t="str">
+        <f t="shared" si="38"/>
+        <v>""</v>
+      </c>
+      <c r="O141" t="str">
+        <f t="shared" si="39"/>
+        <v>""</v>
+      </c>
+      <c r="P141" s="7" t="str">
+        <f t="shared" si="40"/>
+        <v>functions.add(new Function("Gtin", "Gtin", "RelatedProduct"));</v>
+      </c>
+    </row>
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B142" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="I142" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>"Format"</v>
+      </c>
+      <c r="J142" t="str">
+        <f t="shared" si="34"/>
+        <v>"ExpressionResultLiteral"</v>
+      </c>
+      <c r="K142" t="str">
+        <f t="shared" si="35"/>
+        <v>"Gtin"</v>
+      </c>
+      <c r="L142" t="str">
+        <f t="shared" si="36"/>
+        <v>""</v>
+      </c>
+      <c r="M142" t="str">
+        <f t="shared" si="37"/>
+        <v>""</v>
+      </c>
+      <c r="N142" t="str">
+        <f t="shared" si="38"/>
+        <v>""</v>
+      </c>
+      <c r="O142" t="str">
+        <f t="shared" si="39"/>
+        <v>""</v>
+      </c>
+      <c r="P142" s="7" t="str">
+        <f t="shared" si="40"/>
+        <v>functions.add(new Function("Format", "ExpressionResultLiteral", "Gtin"));</v>
+      </c>
+    </row>
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D143" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="I143" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>"HasValue"</v>
+      </c>
+      <c r="J143" t="str">
+        <f t="shared" si="34"/>
+        <v>"ExpressionResultLiteral"</v>
+      </c>
+      <c r="K143" t="str">
+        <f t="shared" si="35"/>
+        <v>"Int32"</v>
+      </c>
+      <c r="L143" t="str">
+        <f t="shared" si="36"/>
+        <v>""</v>
+      </c>
+      <c r="M143" t="str">
+        <f t="shared" si="37"/>
+        <v>""</v>
+      </c>
+      <c r="N143" t="str">
+        <f t="shared" si="38"/>
+        <v>""</v>
+      </c>
+      <c r="O143" t="str">
+        <f t="shared" si="39"/>
+        <v>""</v>
+      </c>
+      <c r="P143" s="7" t="str">
+        <f t="shared" si="40"/>
+        <v>functions.add(new Function("HasValue", "ExpressionResultLiteral", "Int32"));</v>
+      </c>
+    </row>
+    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D144" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="I144" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>"Height"</v>
+      </c>
+      <c r="J144" t="str">
+        <f t="shared" si="34"/>
+        <v>"Int32"</v>
+      </c>
+      <c r="K144" t="str">
+        <f t="shared" si="35"/>
+        <v>"ProductPackage"</v>
+      </c>
+      <c r="L144" t="str">
+        <f t="shared" si="36"/>
+        <v>""</v>
+      </c>
+      <c r="M144" t="str">
+        <f t="shared" si="37"/>
+        <v>""</v>
+      </c>
+      <c r="N144" t="str">
+        <f t="shared" si="38"/>
+        <v>""</v>
+      </c>
+      <c r="O144" t="str">
+        <f t="shared" si="39"/>
+        <v>""</v>
+      </c>
+      <c r="P144" s="7" t="str">
+        <f t="shared" si="40"/>
+        <v>functions.add(new Function("Height", "Int32", "ProductPackage"));</v>
+      </c>
+    </row>
+    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D145" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="I145" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>"Width"</v>
+      </c>
+      <c r="J145" t="str">
+        <f t="shared" ref="J145:J151" si="41">CONCATENATE("""",B145,"""")</f>
+        <v>"Int32"</v>
+      </c>
+      <c r="K145" t="str">
+        <f t="shared" ref="K145:K150" si="42">CONCATENATE("""",D145,"""")</f>
+        <v>"ProductPackage"</v>
+      </c>
+      <c r="L145" t="str">
+        <f t="shared" ref="L145:L150" si="43">CONCATENATE("""",E145,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="M145" t="str">
+        <f t="shared" ref="M145:M150" si="44">CONCATENATE("""",F145,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="N145" t="str">
+        <f t="shared" ref="N145:N150" si="45">CONCATENATE("""",G145,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="O145" t="str">
+        <f t="shared" ref="O145:O150" si="46">CONCATENATE("""",H145,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="P145" s="7" t="str">
+        <f t="shared" ref="P145:P150" si="47">SUBSTITUTE(CONCATENATE($Q$1,I145,$P$1,J145,$P$1,K145,$P$1,L145,$P$1,M145,$P$1,N145,$P$1,O145,$R$1),", """"","")</f>
+        <v>functions.add(new Function("Width", "Int32", "ProductPackage"));</v>
+      </c>
+    </row>
+    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D146" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="I146" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>"Weight"</v>
+      </c>
+      <c r="J146" t="str">
+        <f t="shared" si="41"/>
+        <v>"Int32"</v>
+      </c>
+      <c r="K146" t="str">
+        <f t="shared" si="42"/>
+        <v>"ProductPackage"</v>
+      </c>
+      <c r="L146" t="str">
+        <f t="shared" si="43"/>
+        <v>""</v>
+      </c>
+      <c r="M146" t="str">
+        <f t="shared" si="44"/>
+        <v>""</v>
+      </c>
+      <c r="N146" t="str">
+        <f t="shared" si="45"/>
+        <v>""</v>
+      </c>
+      <c r="O146" t="str">
+        <f t="shared" si="46"/>
+        <v>""</v>
+      </c>
+      <c r="P146" s="7" t="str">
+        <f t="shared" si="47"/>
+        <v>functions.add(new Function("Weight", "Int32", "ProductPackage"));</v>
+      </c>
+    </row>
+    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B147" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D147" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="I147" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>"Package"</v>
+      </c>
+      <c r="J147" t="str">
+        <f t="shared" si="41"/>
+        <v>"ProductPackage"</v>
+      </c>
+      <c r="K147" t="str">
+        <f t="shared" si="42"/>
+        <v>"RelatedProduct"</v>
+      </c>
+      <c r="L147" t="str">
+        <f t="shared" si="43"/>
+        <v>""</v>
+      </c>
+      <c r="M147" t="str">
+        <f t="shared" si="44"/>
+        <v>""</v>
+      </c>
+      <c r="N147" t="str">
+        <f t="shared" si="45"/>
+        <v>""</v>
+      </c>
+      <c r="O147" t="str">
+        <f t="shared" si="46"/>
+        <v>""</v>
+      </c>
+      <c r="P147" s="7" t="str">
+        <f t="shared" si="47"/>
+        <v>functions.add(new Function("Package", "ProductPackage", "RelatedProduct"));</v>
+      </c>
+    </row>
+    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B148" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D148" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="I148" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>"IsBiggerThan()"</v>
+      </c>
+      <c r="J148" t="str">
+        <f t="shared" si="41"/>
+        <v>"ExpressionResultLiteral"</v>
+      </c>
+      <c r="K148" t="str">
+        <f t="shared" si="42"/>
+        <v>"ProductPackage"</v>
+      </c>
+      <c r="L148" t="str">
+        <f t="shared" si="43"/>
+        <v>""</v>
+      </c>
+      <c r="M148" t="str">
+        <f t="shared" si="44"/>
+        <v>""</v>
+      </c>
+      <c r="N148" t="str">
+        <f t="shared" si="45"/>
+        <v>""</v>
+      </c>
+      <c r="O148" t="str">
+        <f t="shared" si="46"/>
+        <v>""</v>
+      </c>
+      <c r="P148" s="7" t="str">
+        <f t="shared" si="47"/>
+        <v>functions.add(new Function("IsBiggerThan()", "ExpressionResultLiteral", "ProductPackage"));</v>
+      </c>
+    </row>
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B149" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D149" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="I149" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>"BulletFeatures[]"</v>
+      </c>
+      <c r="J149" t="str">
+        <f t="shared" si="41"/>
+        <v>"ExpressionResultLiteral"</v>
+      </c>
+      <c r="K149" t="str">
+        <f t="shared" si="42"/>
+        <v>"TemplexGenerator"</v>
+      </c>
+      <c r="L149" t="str">
+        <f t="shared" si="43"/>
+        <v>""</v>
+      </c>
+      <c r="M149" t="str">
+        <f t="shared" si="44"/>
+        <v>""</v>
+      </c>
+      <c r="N149" t="str">
+        <f t="shared" si="45"/>
+        <v>""</v>
+      </c>
+      <c r="O149" t="str">
+        <f t="shared" si="46"/>
+        <v>""</v>
+      </c>
+      <c r="P149" s="7" t="str">
+        <f t="shared" si="47"/>
+        <v>functions.add(new Function("BulletFeatures[]", "ExpressionResultLiteral", "TemplexGenerator"));</v>
+      </c>
+    </row>
+    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B150" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D150" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="I150" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>"Ksp[]"</v>
+      </c>
+      <c r="J150" t="str">
+        <f t="shared" si="41"/>
+        <v>"ExpressionResultLiteral"</v>
+      </c>
+      <c r="K150" t="str">
+        <f t="shared" si="42"/>
+        <v>"DigitalContent"</v>
+      </c>
+      <c r="L150" t="str">
+        <f t="shared" si="43"/>
+        <v>""</v>
+      </c>
+      <c r="M150" t="str">
+        <f t="shared" si="44"/>
+        <v>""</v>
+      </c>
+      <c r="N150" t="str">
+        <f t="shared" si="45"/>
+        <v>""</v>
+      </c>
+      <c r="O150" t="str">
+        <f t="shared" si="46"/>
+        <v>""</v>
+      </c>
+      <c r="P150" s="7" t="str">
+        <f t="shared" si="47"/>
+        <v>functions.add(new Function("Ksp[]", "ExpressionResultLiteral", "DigitalContent"));</v>
+      </c>
+    </row>
+    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B151" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="I151" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>"\"\""</v>
+      </c>
+      <c r="J151" t="str">
+        <f t="shared" si="41"/>
+        <v>"You can invoke nothing on it"</v>
+      </c>
+      <c r="K151" t="str">
+        <f t="shared" ref="K151" si="48">CONCATENATE("""",D151,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="L151" t="str">
+        <f t="shared" ref="L151" si="49">CONCATENATE("""",E151,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="M151" t="str">
+        <f t="shared" ref="M151" si="50">CONCATENATE("""",F151,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="N151" t="str">
+        <f t="shared" ref="N151" si="51">CONCATENATE("""",G151,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="O151" t="str">
+        <f t="shared" ref="O151" si="52">CONCATENATE("""",H151,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="P151" s="7" t="str">
+        <f t="shared" ref="P151" si="53">SUBSTITUTE(CONCATENATE($Q$1,I151,$P$1,J151,$P$1,K151,$P$1,L151,$P$1,M151,$P$1,N151,$P$1,O151,$R$1),", """"","")</f>
+        <v>functions.add(new Function("\"\"", "You can invoke nothing on it"));</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H135"/>
+  <autoFilter ref="A1:H151"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add fex changes to checks
</commit_message>
<xml_diff>
--- a/membersOf_v2.xlsx
+++ b/membersOf_v2.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$151</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$154</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="193">
   <si>
     <t>AltCats</t>
   </si>
@@ -589,6 +589,15 @@
   </si>
   <si>
     <t>\"\"</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Day</t>
   </si>
 </sst>
 </file>
@@ -959,9 +968,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R151"/>
+  <dimension ref="A1:R154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1337,7 +1348,7 @@
         <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="C8" t="s">
         <v>159</v>
@@ -1360,7 +1371,7 @@
       </c>
       <c r="J8" t="str">
         <f t="shared" si="2"/>
-        <v>"Int32"</v>
+        <v>"ExpressionResultNumeric"</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="3"/>
@@ -1384,7 +1395,7 @@
       </c>
       <c r="P8" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>functions.add(new Function("Count", "Int32", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "PdmMultivalueAttribute"));</v>
+        <v>functions.add(new Function("Count", "ExpressionResultNumeric", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "PdmMultivalueAttribute"));</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1392,7 +1403,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="C9" t="s">
         <v>159</v>
@@ -1409,7 +1420,7 @@
       </c>
       <c r="J9" t="str">
         <f t="shared" si="2"/>
-        <v>"Int32"</v>
+        <v>"ExpressionResultNumeric"</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="3"/>
@@ -1433,7 +1444,7 @@
       </c>
       <c r="P9" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>functions.add(new Function("Total", "Int32", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
+        <v>functions.add(new Function("Total", "ExpressionResultNumeric", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -3039,9 +3050,6 @@
       <c r="F43" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="G43" s="6" t="s">
-        <v>162</v>
-      </c>
       <c r="I43" s="5" t="str">
         <f t="shared" si="1"/>
         <v>"Pluralize()"</v>
@@ -3064,7 +3072,7 @@
       </c>
       <c r="N43" t="str">
         <f t="shared" si="6"/>
-        <v>"Int32"</v>
+        <v>""</v>
       </c>
       <c r="O43" t="str">
         <f t="shared" si="7"/>
@@ -3072,7 +3080,7 @@
       </c>
       <c r="P43" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>functions.add(new Function("Pluralize()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "Int32"));</v>
+        <v>functions.add(new Function("Pluralize()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -4679,7 +4687,7 @@
         <v>9</v>
       </c>
       <c r="B77" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="C77" t="s">
         <v>162</v>
@@ -4693,7 +4701,7 @@
       </c>
       <c r="J77" t="str">
         <f t="shared" si="10"/>
-        <v>"Int32"</v>
+        <v>"ExpressionResultNumeric"</v>
       </c>
       <c r="K77" t="str">
         <f t="shared" si="11"/>
@@ -4717,7 +4725,7 @@
       </c>
       <c r="P77" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>functions.add(new Function("CategoryKey", "Int32", "RelatedProduct"));</v>
+        <v>functions.add(new Function("CategoryKey", "ExpressionResultNumeric", "RelatedProduct"));</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
@@ -4725,7 +4733,7 @@
         <v>32</v>
       </c>
       <c r="B78" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="C78" t="s">
         <v>162</v>
@@ -4748,7 +4756,7 @@
       </c>
       <c r="J78" t="str">
         <f t="shared" si="10"/>
-        <v>"Int32"</v>
+        <v>"ExpressionResultNumeric"</v>
       </c>
       <c r="K78" t="str">
         <f t="shared" si="11"/>
@@ -4772,7 +4780,7 @@
       </c>
       <c r="P78" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>functions.add(new Function("Length", "Int32", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "ProductPackage"));</v>
+        <v>functions.add(new Function("Length", "ExpressionResultNumeric", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "ProductPackage"));</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
@@ -4780,7 +4788,7 @@
         <v>33</v>
       </c>
       <c r="B79" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="C79" t="s">
         <v>162</v>
@@ -4794,7 +4802,7 @@
       </c>
       <c r="J79" t="str">
         <f t="shared" si="10"/>
-        <v>"Int32"</v>
+        <v>"ExpressionResultNumeric"</v>
       </c>
       <c r="K79" t="str">
         <f t="shared" si="11"/>
@@ -4818,7 +4826,7 @@
       </c>
       <c r="P79" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>functions.add(new Function("LineCount", "Int32", "Specs"));</v>
+        <v>functions.add(new Function("LineCount", "ExpressionResultNumeric", "Specs"));</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
@@ -4826,7 +4834,7 @@
         <v>43</v>
       </c>
       <c r="B80" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="C80" t="s">
         <v>162</v>
@@ -4840,7 +4848,7 @@
       </c>
       <c r="J80" t="str">
         <f t="shared" si="10"/>
-        <v>"Int32"</v>
+        <v>"ExpressionResultNumeric"</v>
       </c>
       <c r="K80" t="str">
         <f t="shared" si="11"/>
@@ -4864,7 +4872,7 @@
       </c>
       <c r="P80" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>functions.add(new Function("NonOemAccessories", "Int32", "Sku"));</v>
+        <v>functions.add(new Function("NonOemAccessories", "ExpressionResultNumeric", "Sku"));</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
@@ -4872,7 +4880,7 @@
         <v>44</v>
       </c>
       <c r="B81" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="C81" t="s">
         <v>162</v>
@@ -4886,7 +4894,7 @@
       </c>
       <c r="J81" t="str">
         <f t="shared" si="10"/>
-        <v>"Int32"</v>
+        <v>"ExpressionResultNumeric"</v>
       </c>
       <c r="K81" t="str">
         <f t="shared" si="11"/>
@@ -4910,7 +4918,7 @@
       </c>
       <c r="P81" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>functions.add(new Function("Order", "Int32", "SpecLine"));</v>
+        <v>functions.add(new Function("Order", "ExpressionResultNumeric", "SpecLine"));</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
@@ -4918,7 +4926,7 @@
         <v>45</v>
       </c>
       <c r="B82" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="C82" t="s">
         <v>162</v>
@@ -4935,7 +4943,7 @@
       </c>
       <c r="J82" t="str">
         <f t="shared" si="10"/>
-        <v>"Int32"</v>
+        <v>"ExpressionResultNumeric"</v>
       </c>
       <c r="K82" t="str">
         <f t="shared" si="11"/>
@@ -4959,7 +4967,7 @@
       </c>
       <c r="P82" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>functions.add(new Function("PackQuantity", "Int32", "Sku", "RelatedProduct"));</v>
+        <v>functions.add(new Function("PackQuantity", "ExpressionResultNumeric", "Sku", "RelatedProduct"));</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
@@ -4967,7 +4975,7 @@
         <v>48</v>
       </c>
       <c r="B83" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="C83" t="s">
         <v>162</v>
@@ -4984,7 +4992,7 @@
       </c>
       <c r="J83" t="str">
         <f t="shared" si="10"/>
-        <v>"Int32"</v>
+        <v>"ExpressionResultNumeric"</v>
       </c>
       <c r="K83" t="str">
         <f t="shared" si="11"/>
@@ -5008,7 +5016,7 @@
       </c>
       <c r="P83" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>functions.add(new Function("ProductId", "Int32", "Sku", "RelatedProduct"));</v>
+        <v>functions.add(new Function("ProductId", "ExpressionResultNumeric", "Sku", "RelatedProduct"));</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
@@ -7521,7 +7529,7 @@
         <v>174</v>
       </c>
       <c r="I137" s="5" t="str">
-        <f t="shared" ref="I137:I139" si="32">CONCATENATE("""",A137,"""")</f>
+        <f t="shared" ref="I137" si="32">CONCATENATE("""",A137,"""")</f>
         <v>"COALESCE()"</v>
       </c>
       <c r="J137" t="str">
@@ -7561,7 +7569,7 @@
         <v>174</v>
       </c>
       <c r="I138" s="5" t="str">
-        <f t="shared" ref="I138:I151" si="33">CONCATENATE("""",A138,"""")</f>
+        <f t="shared" ref="I138:I154" si="33">CONCATENATE("""",A138,"""")</f>
         <v>"NOT NULL"</v>
       </c>
       <c r="J138" t="str">
@@ -7770,7 +7778,7 @@
         <v>128</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="I143" s="5" t="str">
         <f t="shared" si="33"/>
@@ -7782,7 +7790,7 @@
       </c>
       <c r="K143" t="str">
         <f t="shared" si="35"/>
-        <v>"Int32"</v>
+        <v>"ExpressionResultNumeric"</v>
       </c>
       <c r="L143" t="str">
         <f t="shared" si="36"/>
@@ -7802,7 +7810,7 @@
       </c>
       <c r="P143" s="7" t="str">
         <f t="shared" si="40"/>
-        <v>functions.add(new Function("HasValue", "ExpressionResultLiteral", "Int32"));</v>
+        <v>functions.add(new Function("HasValue", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.25">
@@ -7810,7 +7818,7 @@
         <v>181</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="D144" s="4" t="s">
         <v>184</v>
@@ -7821,7 +7829,7 @@
       </c>
       <c r="J144" t="str">
         <f t="shared" si="34"/>
-        <v>"Int32"</v>
+        <v>"ExpressionResultNumeric"</v>
       </c>
       <c r="K144" t="str">
         <f t="shared" si="35"/>
@@ -7845,7 +7853,7 @@
       </c>
       <c r="P144" s="7" t="str">
         <f t="shared" si="40"/>
-        <v>functions.add(new Function("Height", "Int32", "ProductPackage"));</v>
+        <v>functions.add(new Function("Height", "ExpressionResultNumeric", "ProductPackage"));</v>
       </c>
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.25">
@@ -7853,7 +7861,7 @@
         <v>182</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="D145" s="4" t="s">
         <v>184</v>
@@ -7863,8 +7871,8 @@
         <v>"Width"</v>
       </c>
       <c r="J145" t="str">
-        <f t="shared" ref="J145:J151" si="41">CONCATENATE("""",B145,"""")</f>
-        <v>"Int32"</v>
+        <f t="shared" ref="J145:J152" si="41">CONCATENATE("""",B145,"""")</f>
+        <v>"ExpressionResultNumeric"</v>
       </c>
       <c r="K145" t="str">
         <f t="shared" ref="K145:K150" si="42">CONCATENATE("""",D145,"""")</f>
@@ -7888,7 +7896,7 @@
       </c>
       <c r="P145" s="7" t="str">
         <f t="shared" ref="P145:P150" si="47">SUBSTITUTE(CONCATENATE($Q$1,I145,$P$1,J145,$P$1,K145,$P$1,L145,$P$1,M145,$P$1,N145,$P$1,O145,$R$1),", """"","")</f>
-        <v>functions.add(new Function("Width", "Int32", "ProductPackage"));</v>
+        <v>functions.add(new Function("Width", "ExpressionResultNumeric", "ProductPackage"));</v>
       </c>
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.25">
@@ -7896,7 +7904,7 @@
         <v>183</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="D146" s="4" t="s">
         <v>184</v>
@@ -7907,7 +7915,7 @@
       </c>
       <c r="J146" t="str">
         <f t="shared" si="41"/>
-        <v>"Int32"</v>
+        <v>"ExpressionResultNumeric"</v>
       </c>
       <c r="K146" t="str">
         <f t="shared" si="42"/>
@@ -7931,7 +7939,7 @@
       </c>
       <c r="P146" s="7" t="str">
         <f t="shared" si="47"/>
-        <v>functions.add(new Function("Weight", "Int32", "ProductPackage"));</v>
+        <v>functions.add(new Function("Weight", "ExpressionResultNumeric", "ProductPackage"));</v>
       </c>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.25">
@@ -8142,12 +8150,141 @@
         <v>""</v>
       </c>
       <c r="P151" s="7" t="str">
-        <f t="shared" ref="P151" si="53">SUBSTITUTE(CONCATENATE($Q$1,I151,$P$1,J151,$P$1,K151,$P$1,L151,$P$1,M151,$P$1,N151,$P$1,O151,$R$1),", """"","")</f>
+        <f t="shared" ref="P151:P154" si="53">SUBSTITUTE(CONCATENATE($Q$1,I151,$P$1,J151,$P$1,K151,$P$1,L151,$P$1,M151,$P$1,N151,$P$1,O151,$R$1),", """"","")</f>
         <v>functions.add(new Function("\"\"", "You can invoke nothing on it"));</v>
       </c>
     </row>
+    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D152" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="I152" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>"Year"</v>
+      </c>
+      <c r="J152" t="str">
+        <f t="shared" ref="J152:J154" si="54">CONCATENATE("""",B152,"""")</f>
+        <v>"ExpressionResultNumeric"</v>
+      </c>
+      <c r="K152" t="str">
+        <f t="shared" ref="K152:K154" si="55">CONCATENATE("""",D152,"""")</f>
+        <v>"DateTime"</v>
+      </c>
+      <c r="L152" t="str">
+        <f t="shared" ref="L152:L154" si="56">CONCATENATE("""",E152,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="M152" t="str">
+        <f t="shared" ref="M152:M154" si="57">CONCATENATE("""",F152,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="N152" t="str">
+        <f t="shared" ref="N152:N154" si="58">CONCATENATE("""",G152,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="O152" t="str">
+        <f t="shared" ref="O152:O154" si="59">CONCATENATE("""",H152,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="P152" s="7" t="str">
+        <f t="shared" si="53"/>
+        <v>functions.add(new Function("Year", "ExpressionResultNumeric", "DateTime"));</v>
+      </c>
+    </row>
+    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D153" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="I153" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>"Month"</v>
+      </c>
+      <c r="J153" t="str">
+        <f t="shared" si="54"/>
+        <v>"ExpressionResultNumeric"</v>
+      </c>
+      <c r="K153" t="str">
+        <f t="shared" si="55"/>
+        <v>"DateTime"</v>
+      </c>
+      <c r="L153" t="str">
+        <f t="shared" si="56"/>
+        <v>""</v>
+      </c>
+      <c r="M153" t="str">
+        <f t="shared" si="57"/>
+        <v>""</v>
+      </c>
+      <c r="N153" t="str">
+        <f t="shared" si="58"/>
+        <v>""</v>
+      </c>
+      <c r="O153" t="str">
+        <f t="shared" si="59"/>
+        <v>""</v>
+      </c>
+      <c r="P153" s="7" t="str">
+        <f t="shared" si="53"/>
+        <v>functions.add(new Function("Month", "ExpressionResultNumeric", "DateTime"));</v>
+      </c>
+    </row>
+    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D154" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="I154" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>"Day"</v>
+      </c>
+      <c r="J154" t="str">
+        <f t="shared" si="54"/>
+        <v>"ExpressionResultNumeric"</v>
+      </c>
+      <c r="K154" t="str">
+        <f t="shared" si="55"/>
+        <v>"DateTime"</v>
+      </c>
+      <c r="L154" t="str">
+        <f t="shared" si="56"/>
+        <v>""</v>
+      </c>
+      <c r="M154" t="str">
+        <f t="shared" si="57"/>
+        <v>""</v>
+      </c>
+      <c r="N154" t="str">
+        <f t="shared" si="58"/>
+        <v>""</v>
+      </c>
+      <c r="O154" t="str">
+        <f t="shared" si="59"/>
+        <v>""</v>
+      </c>
+      <c r="P154" s="7" t="str">
+        <f t="shared" si="53"/>
+        <v>functions.add(new Function("Day", "ExpressionResultNumeric", "DateTime"));</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H151"/>
+  <autoFilter ref="A1:H154"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add few changes to check membersOf
</commit_message>
<xml_diff>
--- a/membersOf_v2.xlsx
+++ b/membersOf_v2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="255" windowWidth="20115" windowHeight="7815"/>
@@ -14,12 +14,310 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$154</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Valerii</author>
+  </authors>
+  <commentList>
+    <comment ref="E104" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Valerii:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+PdmMultivalueAttribute</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F104" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Valerii:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+PdmRepeatingAttribute</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E105" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Valerii:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+PdmMultivalueAttribute</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F105" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Valerii:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+PdmRepeatingAttribute</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E115" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Valerii:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+PdmMultivalueAttribute</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F115" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Valerii:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+PdmRepeatingAttribute</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E116" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Valerii:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+PdmMultivalueAttribute</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F116" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Valerii:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+PdmRepeatingAttribute</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E117" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Valerii:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+PdmMultivalueAttribute</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F117" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Valerii:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+PdmRepeatingAttribute</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E118" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Valerii:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+PdmMultivalueAttribute</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F118" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Valerii:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+PdmRepeatingAttribute</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="193">
   <si>
     <t>AltCats</t>
   </si>
@@ -604,13 +902,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -967,11 +1278,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5973,12 +6284,8 @@
       <c r="D104" t="s">
         <v>145</v>
       </c>
-      <c r="E104" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F104" t="s">
-        <v>133</v>
-      </c>
+      <c r="E104" s="6"/>
+      <c r="F104" s="4"/>
       <c r="I104" s="5" t="str">
         <f t="shared" si="9"/>
         <v>"Invariant"</v>
@@ -5993,11 +6300,11 @@
       </c>
       <c r="L104" t="str">
         <f t="shared" si="12"/>
-        <v>"PdmMultivalueAttribute"</v>
+        <v>""</v>
       </c>
       <c r="M104" t="str">
         <f t="shared" si="13"/>
-        <v>"PdmRepeatingAttribute"</v>
+        <v>""</v>
       </c>
       <c r="N104" t="str">
         <f t="shared" si="14"/>
@@ -6009,7 +6316,7 @@
       </c>
       <c r="P104" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>functions.add(new Function("Invariant", "ExpressionResultLiteral", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
+        <v>functions.add(new Function("Invariant", "ExpressionResultLiteral", "PdmAttribute"));</v>
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
@@ -6025,12 +6332,8 @@
       <c r="D105" t="s">
         <v>145</v>
       </c>
-      <c r="E105" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F105" t="s">
-        <v>133</v>
-      </c>
+      <c r="E105" s="6"/>
+      <c r="F105" s="4"/>
       <c r="I105" s="5" t="str">
         <f t="shared" si="9"/>
         <v>"InvariantUnit"</v>
@@ -6045,11 +6348,11 @@
       </c>
       <c r="L105" t="str">
         <f t="shared" si="12"/>
-        <v>"PdmMultivalueAttribute"</v>
+        <v>""</v>
       </c>
       <c r="M105" t="str">
         <f t="shared" si="13"/>
-        <v>"PdmRepeatingAttribute"</v>
+        <v>""</v>
       </c>
       <c r="N105" t="str">
         <f t="shared" si="14"/>
@@ -6061,7 +6364,7 @@
       </c>
       <c r="P105" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>functions.add(new Function("InvariantUnit", "ExpressionResultLiteral", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
+        <v>functions.add(new Function("InvariantUnit", "ExpressionResultLiteral", "PdmAttribute"));</v>
       </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
@@ -6515,12 +6818,8 @@
       <c r="D115" t="s">
         <v>145</v>
       </c>
-      <c r="E115" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F115" t="s">
-        <v>133</v>
-      </c>
+      <c r="E115" s="6"/>
+      <c r="F115" s="4"/>
       <c r="I115" s="5" t="str">
         <f t="shared" si="9"/>
         <v>"Unit"</v>
@@ -6535,11 +6834,11 @@
       </c>
       <c r="L115" t="str">
         <f t="shared" si="12"/>
-        <v>"PdmMultivalueAttribute"</v>
+        <v>""</v>
       </c>
       <c r="M115" t="str">
         <f t="shared" si="13"/>
-        <v>"PdmRepeatingAttribute"</v>
+        <v>""</v>
       </c>
       <c r="N115" t="str">
         <f t="shared" si="14"/>
@@ -6551,7 +6850,7 @@
       </c>
       <c r="P115" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>functions.add(new Function("Unit", "ExpressionResultLiteral", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
+        <v>functions.add(new Function("Unit", "ExpressionResultLiteral", "PdmAttribute"));</v>
       </c>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
@@ -6567,12 +6866,8 @@
       <c r="D116" t="s">
         <v>145</v>
       </c>
-      <c r="E116" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F116" t="s">
-        <v>133</v>
-      </c>
+      <c r="E116" s="6"/>
+      <c r="F116" s="4"/>
       <c r="I116" s="5" t="str">
         <f t="shared" si="9"/>
         <v>"UnitUSM"</v>
@@ -6587,11 +6882,11 @@
       </c>
       <c r="L116" t="str">
         <f t="shared" si="12"/>
-        <v>"PdmMultivalueAttribute"</v>
+        <v>""</v>
       </c>
       <c r="M116" t="str">
         <f t="shared" si="13"/>
-        <v>"PdmRepeatingAttribute"</v>
+        <v>""</v>
       </c>
       <c r="N116" t="str">
         <f t="shared" si="14"/>
@@ -6603,7 +6898,7 @@
       </c>
       <c r="P116" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>functions.add(new Function("UnitUSM", "ExpressionResultLiteral", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
+        <v>functions.add(new Function("UnitUSM", "ExpressionResultLiteral", "PdmAttribute"));</v>
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
@@ -6619,12 +6914,8 @@
       <c r="D117" t="s">
         <v>145</v>
       </c>
-      <c r="E117" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F117" t="s">
-        <v>133</v>
-      </c>
+      <c r="E117" s="6"/>
+      <c r="F117" s="4"/>
       <c r="G117" s="4" t="s">
         <v>178</v>
       </c>
@@ -6642,11 +6933,11 @@
       </c>
       <c r="L117" t="str">
         <f t="shared" si="12"/>
-        <v>"PdmMultivalueAttribute"</v>
+        <v>""</v>
       </c>
       <c r="M117" t="str">
         <f t="shared" si="13"/>
-        <v>"PdmRepeatingAttribute"</v>
+        <v>""</v>
       </c>
       <c r="N117" t="str">
         <f t="shared" si="14"/>
@@ -6658,7 +6949,7 @@
       </c>
       <c r="P117" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>functions.add(new Function("Value", "ExpressionResultLiteral", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute", "Gtin"));</v>
+        <v>functions.add(new Function("Value", "ExpressionResultLiteral", "PdmAttribute", "Gtin"));</v>
       </c>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.25">
@@ -6674,12 +6965,8 @@
       <c r="D118" t="s">
         <v>145</v>
       </c>
-      <c r="E118" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F118" t="s">
-        <v>133</v>
-      </c>
+      <c r="E118" s="6"/>
+      <c r="F118" s="4"/>
       <c r="I118" s="5" t="str">
         <f t="shared" si="9"/>
         <v>"ValueUSM"</v>
@@ -6694,11 +6981,11 @@
       </c>
       <c r="L118" t="str">
         <f t="shared" si="12"/>
-        <v>"PdmMultivalueAttribute"</v>
+        <v>""</v>
       </c>
       <c r="M118" t="str">
         <f t="shared" si="13"/>
-        <v>"PdmRepeatingAttribute"</v>
+        <v>""</v>
       </c>
       <c r="N118" t="str">
         <f t="shared" si="14"/>
@@ -6710,7 +6997,7 @@
       </c>
       <c r="P118" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>functions.add(new Function("ValueUSM", "ExpressionResultLiteral", "PdmAttribute", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
+        <v>functions.add(new Function("ValueUSM", "ExpressionResultLiteral", "PdmAttribute"));</v>
       </c>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.25">
@@ -7871,7 +8158,7 @@
         <v>"Width"</v>
       </c>
       <c r="J145" t="str">
-        <f t="shared" ref="J145:J152" si="41">CONCATENATE("""",B145,"""")</f>
+        <f t="shared" ref="J145:J151" si="41">CONCATENATE("""",B145,"""")</f>
         <v>"ExpressionResultNumeric"</v>
       </c>
       <c r="K145" t="str">
@@ -8287,6 +8574,7 @@
   <autoFilter ref="A1:H154"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
add bug fixed, add updater
</commit_message>
<xml_diff>
--- a/membersOf_v2.xlsx
+++ b/membersOf_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="255" windowWidth="20115" windowHeight="7815"/>
+    <workbookView xWindow="240" yWindow="315" windowWidth="20115" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -317,7 +317,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="194">
   <si>
     <t>AltCats</t>
   </si>
@@ -896,6 +896,9 @@
   </si>
   <si>
     <t>Day</t>
+  </si>
+  <si>
+    <t>ToString()</t>
   </si>
 </sst>
 </file>
@@ -1279,10 +1282,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R154"/>
+  <dimension ref="A1:R155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F128" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P154"/>
+    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2688,8 +2691,8 @@
       <c r="A30" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B30" t="s">
-        <v>160</v>
+      <c r="B30" s="4" t="s">
+        <v>126</v>
       </c>
       <c r="C30" t="s">
         <v>160</v>
@@ -2709,7 +2712,7 @@
       </c>
       <c r="J30" t="str">
         <f t="shared" si="2"/>
-        <v>"ExpressionResult"</v>
+        <v>"ExpressionResultList"</v>
       </c>
       <c r="K30" t="str">
         <f t="shared" si="3"/>
@@ -2733,7 +2736,7 @@
       </c>
       <c r="P30" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>functions.add(new Function("ExtractDecimals()", "ExpressionResult", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
+        <v>functions.add(new Function("ExtractDecimals()", "ExpressionResultList", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric"));</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -5565,13 +5568,19 @@
         <v>113</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>127</v>
+        <v>160</v>
       </c>
       <c r="C89" t="s">
         <v>164</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>127</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="I89" s="5" t="str">
         <f t="shared" si="9"/>
@@ -5579,7 +5588,7 @@
       </c>
       <c r="J89" t="str">
         <f t="shared" si="10"/>
-        <v>"ExpressionResultNumeric"</v>
+        <v>"ExpressionResult"</v>
       </c>
       <c r="K89" t="str">
         <f t="shared" si="11"/>
@@ -5587,11 +5596,11 @@
       </c>
       <c r="L89" t="str">
         <f t="shared" si="12"/>
-        <v>""</v>
+        <v>"ExpressionResultList"</v>
       </c>
       <c r="M89" t="str">
         <f t="shared" si="13"/>
-        <v>""</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="N89" t="str">
         <f t="shared" si="14"/>
@@ -5603,7 +5612,7 @@
       </c>
       <c r="P89" s="7" t="str">
         <f t="shared" si="16"/>
-        <v>functions.add(new Function("MultiplyBy()", "ExpressionResultNumeric", "ExpressionResultNumeric"));</v>
+        <v>functions.add(new Function("MultiplyBy()", "ExpressionResult", "ExpressionResultNumeric", "ExpressionResultList", "ExpressionResultLiteral"));</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
@@ -8568,6 +8577,58 @@
       <c r="P154" s="7" t="str">
         <f t="shared" si="53"/>
         <v>functions.add(new Function("Day", "ExpressionResultNumeric", "DateTime"));</v>
+      </c>
+    </row>
+    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B155" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D155" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E155" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F155" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G155" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="I155" s="5" t="str">
+        <f t="shared" ref="I155" si="60">CONCATENATE("""",A155,"""")</f>
+        <v>"ToString()"</v>
+      </c>
+      <c r="J155" t="str">
+        <f t="shared" ref="J155" si="61">CONCATENATE("""",B155,"""")</f>
+        <v>"ExpressionResultLiteral"</v>
+      </c>
+      <c r="K155" t="str">
+        <f t="shared" ref="K155" si="62">CONCATENATE("""",D155,"""")</f>
+        <v>"ExpressionResultList"</v>
+      </c>
+      <c r="L155" t="str">
+        <f t="shared" ref="L155" si="63">CONCATENATE("""",E155,"""")</f>
+        <v>"ExpressionResultLiteral"</v>
+      </c>
+      <c r="M155" t="str">
+        <f t="shared" ref="M155" si="64">CONCATENATE("""",F155,"""")</f>
+        <v>"ExpressionResultNumeric"</v>
+      </c>
+      <c r="N155" t="str">
+        <f t="shared" ref="N155" si="65">CONCATENATE("""",G155,"""")</f>
+        <v>"DateTimeOffset"</v>
+      </c>
+      <c r="O155" t="str">
+        <f t="shared" ref="O155" si="66">CONCATENATE("""",H155,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="P155" s="7" t="str">
+        <f t="shared" ref="P155" si="67">SUBSTITUTE(CONCATENATE($Q$1,I155,$P$1,J155,$P$1,K155,$P$1,L155,$P$1,M155,$P$1,N155,$P$1,O155,$R$1),", """"","")</f>
+        <v>functions.add(new Function("ToString()", "ExpressionResultLiteral", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "DateTimeOffset"));</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new attr, add DECODE, add bug fixes, change file filter
</commit_message>
<xml_diff>
--- a/membersOf_v2.xlsx
+++ b/membersOf_v2.xlsx
@@ -317,7 +317,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="195">
   <si>
     <t>AltCats</t>
   </si>
@@ -899,6 +899,9 @@
   </si>
   <si>
     <t>ToString()</t>
+  </si>
+  <si>
+    <t>DECODE()</t>
   </si>
 </sst>
 </file>
@@ -1282,10 +1285,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R155"/>
+  <dimension ref="A1:R156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="B156" sqref="B156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8599,7 +8602,7 @@
         <v>158</v>
       </c>
       <c r="I155" s="5" t="str">
-        <f t="shared" ref="I155" si="60">CONCATENATE("""",A155,"""")</f>
+        <f t="shared" ref="I155:I156" si="60">CONCATENATE("""",A155,"""")</f>
         <v>"ToString()"</v>
       </c>
       <c r="J155" t="str">
@@ -8629,6 +8632,46 @@
       <c r="P155" s="7" t="str">
         <f t="shared" ref="P155" si="67">SUBSTITUTE(CONCATENATE($Q$1,I155,$P$1,J155,$P$1,K155,$P$1,L155,$P$1,M155,$P$1,N155,$P$1,O155,$R$1),", """"","")</f>
         <v>functions.add(new Function("ToString()", "ExpressionResultLiteral", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "DateTimeOffset"));</v>
+      </c>
+    </row>
+    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="I156" s="5" t="str">
+        <f t="shared" si="60"/>
+        <v>"DECODE()"</v>
+      </c>
+      <c r="J156" t="str">
+        <f t="shared" ref="J156" si="68">CONCATENATE("""",B156,"""")</f>
+        <v>"You can invoke nothing on it"</v>
+      </c>
+      <c r="K156" t="str">
+        <f t="shared" ref="K156" si="69">CONCATENATE("""",D156,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="L156" t="str">
+        <f t="shared" ref="L156" si="70">CONCATENATE("""",E156,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="M156" t="str">
+        <f t="shared" ref="M156" si="71">CONCATENATE("""",F156,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="N156" t="str">
+        <f t="shared" ref="N156" si="72">CONCATENATE("""",G156,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="O156" t="str">
+        <f t="shared" ref="O156" si="73">CONCATENATE("""",H156,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="P156" s="7" t="str">
+        <f t="shared" ref="P156" si="74">SUBSTITUTE(CONCATENATE($Q$1,I156,$P$1,J156,$P$1,K156,$P$1,L156,$P$1,M156,$P$1,N156,$P$1,O156,$R$1),", """"","")</f>
+        <v>functions.add(new Function("DECODE()", "You can invoke nothing on it"));</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new attributes, fixed attributes, change members of  Values funciton, fix check of 0 parameters
</commit_message>
<xml_diff>
--- a/membersOf_v2.xlsx
+++ b/membersOf_v2.xlsx
@@ -317,7 +317,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="195">
   <si>
     <t>AltCats</t>
   </si>
@@ -1287,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="B156" sqref="B156"/>
+    <sheetView tabSelected="1" topLeftCell="F35" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3838,6 +3838,9 @@
       <c r="F52" t="s">
         <v>133</v>
       </c>
+      <c r="G52" s="4" t="s">
+        <v>144</v>
+      </c>
       <c r="I52" s="5" t="str">
         <f t="shared" si="1"/>
         <v>"Values"</v>
@@ -3860,7 +3863,7 @@
       </c>
       <c r="N52" t="str">
         <f t="shared" si="6"/>
-        <v>""</v>
+        <v>"DigitalContentItem"</v>
       </c>
       <c r="O52" t="str">
         <f t="shared" si="7"/>
@@ -3868,7 +3871,7 @@
       </c>
       <c r="P52" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>functions.add(new Function("Values", "ExpressionResultList", "PdmAttributeSet", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
+        <v>functions.add(new Function("Values", "ExpressionResultList", "PdmAttributeSet", "PdmMultivalueAttribute", "PdmRepeatingAttribute", "DigitalContentItem"));</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix issue with invoking Count function on the Repeating Attribute
</commit_message>
<xml_diff>
--- a/membersOf_v2.xlsx
+++ b/membersOf_v2.xlsx
@@ -317,7 +317,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="195">
   <si>
     <t>AltCats</t>
   </si>
@@ -1287,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F35" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1682,6 +1682,9 @@
       <c r="G8" s="2" t="s">
         <v>132</v>
       </c>
+      <c r="H8" t="s">
+        <v>133</v>
+      </c>
       <c r="I8" s="5" t="str">
         <f t="shared" si="1"/>
         <v>"Count"</v>
@@ -1708,11 +1711,11 @@
       </c>
       <c r="O8" t="str">
         <f t="shared" si="7"/>
-        <v>""</v>
+        <v>"PdmRepeatingAttribute"</v>
       </c>
       <c r="P8" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>functions.add(new Function("Count", "ExpressionResultNumeric", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "PdmMultivalueAttribute"));</v>
+        <v>functions.add(new Function("Count", "ExpressionResultNumeric", "ExpressionResultList", "ExpressionResultLiteral", "ExpressionResultNumeric", "PdmMultivalueAttribute", "PdmRepeatingAttribute"));</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed issue with invoking functions: Round(), AtLeast() and AtMost() on ExpressionResultLiteral
</commit_message>
<xml_diff>
--- a/membersOf_v2.xlsx
+++ b/membersOf_v2.xlsx
@@ -317,7 +317,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="196">
   <si>
     <t>AltCats</t>
   </si>
@@ -1290,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="G62" workbookViewId="0">
+      <selection activeCell="R86" sqref="R86:R88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5797,6 +5797,9 @@
       <c r="D86" s="2" t="s">
         <v>127</v>
       </c>
+      <c r="E86" s="6" t="s">
+        <v>128</v>
+      </c>
       <c r="J86" s="5" t="str">
         <f t="shared" si="11"/>
         <v>"Round()"</v>
@@ -5811,7 +5814,7 @@
       </c>
       <c r="M86" t="str">
         <f t="shared" si="14"/>
-        <v>""</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="N86" t="str">
         <f t="shared" si="15"/>
@@ -5831,7 +5834,7 @@
       </c>
       <c r="R86" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>functions.add(new Function("Round()", "ExpressionResultNumeric", "ExpressionResultNumeric"));</v>
+        <v>functions.add(new Function("Round()", "ExpressionResultNumeric", "ExpressionResultNumeric", "ExpressionResultLiteral"));</v>
       </c>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.25">
@@ -5847,6 +5850,9 @@
       <c r="D87" s="2" t="s">
         <v>127</v>
       </c>
+      <c r="E87" s="6" t="s">
+        <v>128</v>
+      </c>
       <c r="J87" s="5" t="str">
         <f t="shared" si="11"/>
         <v>"AtLeast()"</v>
@@ -5861,7 +5867,7 @@
       </c>
       <c r="M87" t="str">
         <f t="shared" si="14"/>
-        <v>""</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="N87" t="str">
         <f t="shared" si="15"/>
@@ -5881,7 +5887,7 @@
       </c>
       <c r="R87" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>functions.add(new Function("AtLeast()", "ExpressionResultNumeric", "ExpressionResultNumeric"));</v>
+        <v>functions.add(new Function("AtLeast()", "ExpressionResultNumeric", "ExpressionResultNumeric", "ExpressionResultLiteral"));</v>
       </c>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
@@ -5897,6 +5903,9 @@
       <c r="D88" s="2" t="s">
         <v>127</v>
       </c>
+      <c r="E88" s="6" t="s">
+        <v>128</v>
+      </c>
       <c r="J88" s="5" t="str">
         <f t="shared" si="11"/>
         <v>"AtMost()"</v>
@@ -5911,7 +5920,7 @@
       </c>
       <c r="M88" t="str">
         <f t="shared" si="14"/>
-        <v>""</v>
+        <v>"ExpressionResultLiteral"</v>
       </c>
       <c r="N88" t="str">
         <f t="shared" si="15"/>
@@ -5931,7 +5940,7 @@
       </c>
       <c r="R88" s="7" t="str">
         <f t="shared" si="10"/>
-        <v>functions.add(new Function("AtMost()", "ExpressionResultNumeric", "ExpressionResultNumeric"));</v>
+        <v>functions.add(new Function("AtMost()", "ExpressionResultNumeric", "ExpressionResultNumeric", "ExpressionResultLiteral"));</v>
       </c>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>